<commit_message>
update output phi npq
</commit_message>
<xml_diff>
--- a/02_pam/output/stat_results/pairwise_allmetsxtissues.xlsx
+++ b/02_pam/output/stat_results/pairwise_allmetsxtissues.xlsx
@@ -8,13 +8,13 @@
   <sheets>
     <sheet name="Fv.Fm" r:id="rId3" sheetId="1"/>
     <sheet name="φPSII" r:id="rId4" sheetId="2"/>
-    <sheet name="NPQ" r:id="rId5" sheetId="3"/>
+    <sheet name="ΦNPQ" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="770">
   <si>
     <t/>
   </si>
@@ -1612,814 +1612,718 @@
     <t>0.00250495181779634</t>
   </si>
   <si>
-    <t>2.07907673424472e-06</t>
-  </si>
-  <si>
-    <t>2.76256276330773e-06</t>
-  </si>
-  <si>
-    <t>2.30656060294431e-05</t>
-  </si>
-  <si>
-    <t>1.6654676260957e-05</t>
-  </si>
-  <si>
-    <t>0.000130869554291803</t>
-  </si>
-  <si>
-    <t>4.27076879007475e-09</t>
-  </si>
-  <si>
-    <t>2.87619168756241e-09</t>
-  </si>
-  <si>
-    <t>1.32898698150291e-08</t>
-  </si>
-  <si>
-    <t>4.20619952136152e-09</t>
-  </si>
-  <si>
-    <t>7.55653259979479e-09</t>
-  </si>
-  <si>
-    <t>6.94892103552471e-06</t>
-  </si>
-  <si>
-    <t>5.63910559901493e-06</t>
-  </si>
-  <si>
-    <t>4.34377291029122e-06</t>
-  </si>
-  <si>
-    <t>3.54342862095047e-06</t>
-  </si>
-  <si>
-    <t>9.32144968267827e-06</t>
-  </si>
-  <si>
-    <t>3.65598522359719e-05</t>
-  </si>
-  <si>
-    <t>2.52610565287893e-06</t>
-  </si>
-  <si>
-    <t>8.21550369673415e-05</t>
-  </si>
-  <si>
-    <t>0.000116087733453489</t>
-  </si>
-  <si>
-    <t>0.000700335008014369</t>
-  </si>
-  <si>
-    <t>0.000608203783147263</t>
-  </si>
-  <si>
-    <t>0.000846211795326846</t>
-  </si>
-  <si>
-    <t>0.00238119660835579</t>
-  </si>
-  <si>
-    <t>5.78890758650745e-06</t>
-  </si>
-  <si>
-    <t>3.37954480959651e-06</t>
-  </si>
-  <si>
-    <t>1.2763932957989e-05</t>
-  </si>
-  <si>
-    <t>4.01371217254406e-06</t>
-  </si>
-  <si>
-    <t>5.56903989177536e-06</t>
-  </si>
-  <si>
-    <t>0.00025606830806697</t>
-  </si>
-  <si>
-    <t>0.00020591807840194</t>
-  </si>
-  <si>
-    <t>0.000168203090368367</t>
-  </si>
-  <si>
-    <t>0.00013703379736168</t>
-  </si>
-  <si>
-    <t>0.000335443765679209</t>
-  </si>
-  <si>
-    <t>0.00124421927028259</t>
-  </si>
-  <si>
-    <t>9.74871516610149e-05</t>
-  </si>
-  <si>
-    <t>0.00528131675465276</t>
-  </si>
-  <si>
-    <t>0.00614740448847222</t>
-  </si>
-  <si>
-    <t>0.0197019400097082</t>
-  </si>
-  <si>
-    <t>0.0166200059634158</t>
-  </si>
-  <si>
-    <t>0.0211466746353523</t>
-  </si>
-  <si>
-    <t>0.0403127850334353</t>
-  </si>
-  <si>
-    <t>0.00256097547816217</t>
-  </si>
-  <si>
-    <t>0.00190746506205817</t>
-  </si>
-  <si>
-    <t>0.00392118295104916</t>
-  </si>
-  <si>
-    <t>0.00176778028284485</t>
-  </si>
-  <si>
-    <t>0.00195739488853037</t>
-  </si>
-  <si>
-    <t>0.00222911961184039</t>
-  </si>
-  <si>
-    <t>0.00955784510803099</t>
-  </si>
-  <si>
-    <t>0.00841797827290205</t>
-  </si>
-  <si>
-    <t>0.0074480060992772</t>
-  </si>
-  <si>
-    <t>0.00669069290857137</t>
-  </si>
-  <si>
-    <t>0.0113455383716777</t>
-  </si>
-  <si>
-    <t>0.0287325956377891</t>
-  </si>
-  <si>
-    <t>0.00565670420231387</t>
-  </si>
-  <si>
-    <t>5.28791316228175e-05</t>
-  </si>
-  <si>
-    <t>3.9546325182081e-05</t>
-  </si>
-  <si>
-    <t>5.63353478662892e-05</t>
-  </si>
-  <si>
-    <t>0.000251911942625422</t>
-  </si>
-  <si>
-    <t>1.76622387156217e-08</t>
-  </si>
-  <si>
-    <t>7.92528911797226e-08</t>
-  </si>
-  <si>
-    <t>2.93737690327018e-08</t>
-  </si>
-  <si>
-    <t>1.11114746085186e-08</t>
-  </si>
-  <si>
-    <t>1.57894223144471e-05</t>
-  </si>
-  <si>
-    <t>1.20622411644083e-05</t>
-  </si>
-  <si>
-    <t>9.33043983027274e-06</t>
-  </si>
-  <si>
-    <t>7.49897132467149e-06</t>
-  </si>
-  <si>
-    <t>2.06875339422779e-05</t>
-  </si>
-  <si>
-    <t>8.58677806326628e-05</t>
-  </si>
-  <si>
-    <t>5.25288485002361e-06</t>
-  </si>
-  <si>
-    <t>0.600342999763839</t>
-  </si>
-  <si>
-    <t>0.196197837172752</t>
-  </si>
-  <si>
-    <t>0.000654480058277181</t>
-  </si>
-  <si>
-    <t>0.445191879641434</t>
-  </si>
-  <si>
-    <t>0.000268286295401313</t>
-  </si>
-  <si>
-    <t>0.323289337126215</t>
-  </si>
-  <si>
-    <t>0.00260699980090117</t>
-  </si>
-  <si>
-    <t>0.726887978100326</t>
-  </si>
-  <si>
-    <t>0.00624119581218444</t>
-  </si>
-  <si>
-    <t>0.00242029347679278</t>
-  </si>
-  <si>
-    <t>0.877597651959522</t>
-  </si>
-  <si>
-    <t>1.1228150020061e-05</t>
-  </si>
-  <si>
-    <t>0.00220501951921627</t>
-  </si>
-  <si>
-    <t>0.20678443406375</t>
-  </si>
-  <si>
-    <t>0.000367806974899573</t>
-  </si>
-  <si>
-    <t>8.18175272779636e-06</t>
-  </si>
-  <si>
-    <t>0.000486699403108072</t>
-  </si>
-  <si>
-    <t>0.0445686716637928</t>
-  </si>
-  <si>
-    <t>0.00118662328606453</t>
-  </si>
-  <si>
-    <t>0.00257943264906973</t>
-  </si>
-  <si>
-    <t>0.0722335770587373</t>
-  </si>
-  <si>
-    <t>0.604864236716358</t>
-  </si>
-  <si>
-    <t>0.000997390898428725</t>
-  </si>
-  <si>
-    <t>0.602353069781445</t>
-  </si>
-  <si>
-    <t>0.0246426651804471</t>
-  </si>
-  <si>
-    <t>0.411630634364774</t>
-  </si>
-  <si>
-    <t>0.0203870800252601</t>
-  </si>
-  <si>
-    <t>0.014079578678623</t>
-  </si>
-  <si>
-    <t>0.800374746740521</t>
-  </si>
-  <si>
-    <t>2.2373511837209e-05</t>
-  </si>
-  <si>
-    <t>0.00393266367860221</t>
-  </si>
-  <si>
-    <t>0.0647878784866992</t>
-  </si>
-  <si>
-    <t>7.94469834717513e-05</t>
-  </si>
-  <si>
-    <t>0.000179811321564906</t>
-  </si>
-  <si>
-    <t>0.0028980028980029</t>
-  </si>
-  <si>
-    <t>0.0688540930904962</t>
-  </si>
-  <si>
-    <t>0.0137848259659338</t>
-  </si>
-  <si>
-    <t>0.00490042747447415</t>
-  </si>
-  <si>
-    <t>0.240424774159149</t>
-  </si>
-  <si>
-    <t>0.0249638532514534</t>
-  </si>
-  <si>
-    <t>0.000240799602888593</t>
-  </si>
-  <si>
-    <t>0.262272495076611</t>
-  </si>
-  <si>
-    <t>0.0006980712332225</t>
-  </si>
-  <si>
-    <t>0.000182047917089801</t>
-  </si>
-  <si>
-    <t>0.157452336455632</t>
-  </si>
-  <si>
-    <t>0.000370741156562194</t>
-  </si>
-  <si>
-    <t>0.00015515266284432</t>
-  </si>
-  <si>
-    <t>0.00316934630827</t>
-  </si>
-  <si>
-    <t>0.985354101840775</t>
-  </si>
-  <si>
-    <t>0.000168782045913667</t>
-  </si>
-  <si>
-    <t>0.000187852218468315</t>
-  </si>
-  <si>
-    <t>0.000501559061121037</t>
-  </si>
-  <si>
-    <t>0.0188449569438324</t>
-  </si>
-  <si>
-    <t>0.00500685343673584</t>
-  </si>
-  <si>
-    <t>0.00133803220673666</t>
-  </si>
-  <si>
-    <t>0.214855320118478</t>
-  </si>
-  <si>
-    <t>0.00172653546597966</t>
-  </si>
-  <si>
-    <t>0.0448141167792694</t>
-  </si>
-  <si>
-    <t>0.315968072442553</t>
-  </si>
-  <si>
-    <t>0.00354141780205215</t>
-  </si>
-  <si>
-    <t>0.693877193117093</t>
-  </si>
-  <si>
-    <t>0.431155828929289</t>
-  </si>
-  <si>
-    <t>0.0281625259488343</t>
-  </si>
-  <si>
-    <t>0.0116416916416916</t>
-  </si>
-  <si>
-    <t>0.00116437616437616</t>
-  </si>
-  <si>
-    <t>0.945450748082327</t>
-  </si>
-  <si>
-    <t>0.000413515855636221</t>
-  </si>
-  <si>
-    <t>0.00701176757514786</t>
-  </si>
-  <si>
-    <t>0.567429196483508</t>
-  </si>
-  <si>
-    <t>0.123264970323794</t>
-  </si>
-  <si>
-    <t>0.255018674136321</t>
-  </si>
-  <si>
-    <t>0.134865134865135</t>
-  </si>
-  <si>
-    <t>0.0141625615763547</t>
-  </si>
-  <si>
-    <t>0.0169790826547337</t>
-  </si>
-  <si>
-    <t>0.0195949811728942</t>
-  </si>
-  <si>
-    <t>0.944191501835315</t>
-  </si>
-  <si>
-    <t>0.407383784591097</t>
-  </si>
-  <si>
-    <t>0.40001524687867</t>
-  </si>
-  <si>
-    <t>0.338565379879494</t>
-  </si>
-  <si>
-    <t>0.326832034629018</t>
-  </si>
-  <si>
-    <t>0.673268317117556</t>
-  </si>
-  <si>
-    <t>0.00659627453885827</t>
-  </si>
-  <si>
-    <t>0.00145424196057107</t>
-  </si>
-  <si>
-    <t>0.176595638255302</t>
-  </si>
-  <si>
-    <t>0.0120620935598909</t>
-  </si>
-  <si>
-    <t>0.0963403880070547</t>
-  </si>
-  <si>
-    <t>0.0190876831501832</t>
-  </si>
-  <si>
-    <t>0.432863183104263</t>
-  </si>
-  <si>
-    <t>0.65851588119705</t>
-  </si>
-  <si>
-    <t>0.0220814132104455</t>
-  </si>
-  <si>
-    <t>1.31633877353949e-06</t>
-  </si>
-  <si>
-    <t>0.000188566093494889</t>
-  </si>
-  <si>
-    <t>1.95443287654649e-05</t>
-  </si>
-  <si>
-    <t>0.000245070562875458</t>
-  </si>
-  <si>
-    <t>0.000159042840545842</t>
-  </si>
-  <si>
-    <t>0.00269484196551944</t>
-  </si>
-  <si>
-    <t>0.000620114469402859</t>
-  </si>
-  <si>
-    <t>0.00257623845590698</t>
-  </si>
-  <si>
-    <t>5.13938175376706e-05</t>
-  </si>
-  <si>
-    <t>0.000130521715813253</t>
-  </si>
-  <si>
-    <t>0.000176810752583333</t>
-  </si>
-  <si>
-    <t>0.000796814752641862</t>
-  </si>
-  <si>
-    <t>0.00886605788879028</t>
-  </si>
-  <si>
-    <t>0.00173233669110726</t>
-  </si>
-  <si>
-    <t>0.000985922919111673</t>
-  </si>
-  <si>
-    <t>0.106277110021488</t>
-  </si>
-  <si>
-    <t>1.35345961928652e-05</t>
-  </si>
-  <si>
-    <t>0.0637518697463941</t>
-  </si>
-  <si>
-    <t>0.0453281747557069</t>
-  </si>
-  <si>
-    <t>0.000418625425008667</t>
-  </si>
-  <si>
-    <t>0.00459003988118331</t>
-  </si>
-  <si>
-    <t>0.000121635064588392</t>
-  </si>
-  <si>
-    <t>0.0433764692277697</t>
-  </si>
-  <si>
-    <t>0.396680856257372</t>
-  </si>
-  <si>
-    <t>0.00202435216889078</t>
-  </si>
-  <si>
-    <t>0.191272568809683</t>
-  </si>
-  <si>
-    <t>0.467763796276955</t>
-  </si>
-  <si>
-    <t>1.64853076721174e-06</t>
-  </si>
-  <si>
-    <t>0.000111412306858831</t>
-  </si>
-  <si>
-    <t>0.00121775223344539</t>
-  </si>
-  <si>
-    <t>0.167125912015473</t>
-  </si>
-  <si>
-    <t>0.00361345503265865</t>
-  </si>
-  <si>
-    <t>0.726939081071802</t>
-  </si>
-  <si>
-    <t>0.00818363957872155</t>
-  </si>
-  <si>
-    <t>0.675510840367757</t>
-  </si>
-  <si>
-    <t>8.29905632893306e-07</t>
-  </si>
-  <si>
-    <t>0.395736762884</t>
-  </si>
-  <si>
-    <t>1.29462604924086e-05</t>
-  </si>
-  <si>
-    <t>0.00486995564735691</t>
-  </si>
-  <si>
-    <t>0.368631281978677</t>
-  </si>
-  <si>
-    <t>0.000571632390110858</t>
-  </si>
-  <si>
-    <t>4.80419079582243e-05</t>
-  </si>
-  <si>
-    <t>3.86455024554194e-05</t>
-  </si>
-  <si>
-    <t>0.0439117002354172</t>
-  </si>
-  <si>
-    <t>0.00325106145123811</t>
-  </si>
-  <si>
-    <t>0.002656003099033</t>
-  </si>
-  <si>
-    <t>0.765637087047032</t>
-  </si>
-  <si>
-    <t>6.42327914631204e-05</t>
-  </si>
-  <si>
-    <t>0.00050350168626449</t>
-  </si>
-  <si>
-    <t>0.00133748675992323</t>
-  </si>
-  <si>
-    <t>0.577096359509183</t>
-  </si>
-  <si>
-    <t>0.00854460352780017</t>
-  </si>
-  <si>
-    <t>0.939138571710565</t>
-  </si>
-  <si>
-    <t>0.495925750182711</t>
-  </si>
-  <si>
-    <t>0.0091945372301702</t>
-  </si>
-  <si>
-    <t>0.28278586967736</t>
-  </si>
-  <si>
-    <t>3.83925987423895e-05</t>
-  </si>
-  <si>
-    <t>0.0155052040128474</t>
-  </si>
-  <si>
-    <t>0.00362097940166619</t>
-  </si>
-  <si>
-    <t>0.567326844848566</t>
-  </si>
-  <si>
-    <t>0.00350557788035383</t>
-  </si>
-  <si>
-    <t>0.0304531059520487</t>
-  </si>
-  <si>
-    <t>0.94870621167531</t>
-  </si>
-  <si>
-    <t>0.672004350758738</t>
-  </si>
-  <si>
-    <t>0.0402186425478133</t>
-  </si>
-  <si>
-    <t>0.511458886040916</t>
-  </si>
-  <si>
-    <t>0.000321512174005619</t>
-  </si>
-  <si>
-    <t>0.0384036997811503</t>
-  </si>
-  <si>
-    <t>0.487322747043142</t>
-  </si>
-  <si>
-    <t>0.000898700427802566</t>
-  </si>
-  <si>
-    <t>0.00201652734838777</t>
-  </si>
-  <si>
-    <t>0.0162182175310586</t>
-  </si>
-  <si>
-    <t>0.168959938497167</t>
-  </si>
-  <si>
-    <t>0.00551223229576606</t>
-  </si>
-  <si>
-    <t>0.0482321917855833</t>
-  </si>
-  <si>
-    <t>0.449715772675404</t>
-  </si>
-  <si>
-    <t>0.024361180987687</t>
-  </si>
-  <si>
-    <t>0.00217512899103754</t>
-  </si>
-  <si>
-    <t>0.00145036482320306</t>
-  </si>
-  <si>
-    <t>0.000799531868297403</t>
-  </si>
-  <si>
-    <t>0.239571617193995</t>
-  </si>
-  <si>
-    <t>2.55865721669268e-05</t>
-  </si>
-  <si>
-    <t>0.00322538424142702</t>
-  </si>
-  <si>
-    <t>0.0120931699879068</t>
-  </si>
-  <si>
-    <t>8.61588654600596e-05</t>
-  </si>
-  <si>
-    <t>0.475817778862655</t>
-  </si>
-  <si>
-    <t>0.000136218435408212</t>
-  </si>
-  <si>
-    <t>0.499915420043216</t>
-  </si>
-  <si>
-    <t>0.000233313991941538</t>
-  </si>
-  <si>
-    <t>0.0620647388127965</t>
-  </si>
-  <si>
-    <t>0.486430552369831</t>
-  </si>
-  <si>
-    <t>0.609883943217277</t>
-  </si>
-  <si>
-    <t>0.115418637090464</t>
-  </si>
-  <si>
-    <t>1.90638868977718e-05</t>
-  </si>
-  <si>
-    <t>0.0118228940388452</t>
-  </si>
-  <si>
-    <t>0.000216590859865714</t>
-  </si>
-  <si>
-    <t>0.00865572783381002</t>
-  </si>
-  <si>
-    <t>0.000474716202270382</t>
-  </si>
-  <si>
-    <t>0.0295482366174816</t>
-  </si>
-  <si>
-    <t>0.122943952840452</t>
-  </si>
-  <si>
-    <t>0.112944558628405</t>
-  </si>
-  <si>
-    <t>0.00877568252181255</t>
-  </si>
-  <si>
-    <t>0.0155889200899918</t>
-  </si>
-  <si>
-    <t>0.00798270536912628</t>
-  </si>
-  <si>
-    <t>0.328399491664798</t>
-  </si>
-  <si>
-    <t>0.00267665770761746</t>
-  </si>
-  <si>
-    <t>0.926213644068928</t>
-  </si>
-  <si>
-    <t>0.541062157656585</t>
-  </si>
-  <si>
-    <t>0.00663780663780664</t>
-  </si>
-  <si>
-    <t>0.784412010418202</t>
-  </si>
-  <si>
-    <t>0.00144544997486174</t>
+    <t>1.815891973444e-06</t>
+  </si>
+  <si>
+    <t>2.55792848454419e-06</t>
+  </si>
+  <si>
+    <t>2.0293069451728e-05</t>
+  </si>
+  <si>
+    <t>1.55625663422057e-05</t>
+  </si>
+  <si>
+    <t>4.44398358688729e-05</t>
+  </si>
+  <si>
+    <t>0.000109772141101549</t>
+  </si>
+  <si>
+    <t>3.22751584890857e-09</t>
+  </si>
+  <si>
+    <t>1.61239710194101e-09</t>
+  </si>
+  <si>
+    <t>1.38300851710194e-08</t>
+  </si>
+  <si>
+    <t>1.77630145108456e-08</t>
+  </si>
+  <si>
+    <t>2.26383319989109e-09</t>
+  </si>
+  <si>
+    <t>6.17681869824419e-06</t>
+  </si>
+  <si>
+    <t>4.91614334273096e-06</t>
+  </si>
+  <si>
+    <t>3.18908575885542e-06</t>
+  </si>
+  <si>
+    <t>1.18676261901165e-05</t>
+  </si>
+  <si>
+    <t>2.29645968443539e-06</t>
+  </si>
+  <si>
+    <t>6.94506498074433e-05</t>
+  </si>
+  <si>
+    <t>9.93443103592358e-05</t>
+  </si>
+  <si>
+    <t>0.000588732895025105</t>
+  </si>
+  <si>
+    <t>0.000509370668385833</t>
+  </si>
+  <si>
+    <t>0.00165648231719536</t>
+  </si>
+  <si>
+    <t>0.00212178878633337</t>
+  </si>
+  <si>
+    <t>5.22119368416208e-06</t>
+  </si>
+  <si>
+    <t>3.06231088555659e-06</t>
+  </si>
+  <si>
+    <t>1.25467727214735e-05</t>
+  </si>
+  <si>
+    <t>3.90248978848505e-06</t>
+  </si>
+  <si>
+    <t>7.7309368691066e-06</t>
+  </si>
+  <si>
+    <t>3.93747221251223e-06</t>
+  </si>
+  <si>
+    <t>0.000205929058934976</t>
+  </si>
+  <si>
+    <t>0.000172134643664122</t>
+  </si>
+  <si>
+    <t>0.000115709910040178</t>
+  </si>
+  <si>
+    <t>0.000371332900073929</t>
+  </si>
+  <si>
+    <t>8.29423940317332e-05</t>
+  </si>
+  <si>
+    <t>0.00488828853105069</t>
+  </si>
+  <si>
+    <t>0.00565341662779142</t>
+  </si>
+  <si>
+    <t>0.0186975273817623</t>
+  </si>
+  <si>
+    <t>0.0158190418206006</t>
+  </si>
+  <si>
+    <t>0.0410797225579305</t>
+  </si>
+  <si>
+    <t>0.0390745080113809</t>
+  </si>
+  <si>
+    <t>0.00227785256097841</t>
+  </si>
+  <si>
+    <t>0.00366892402218774</t>
+  </si>
+  <si>
+    <t>0.0015926560182237</t>
+  </si>
+  <si>
+    <t>0.00201570616901119</t>
+  </si>
+  <si>
+    <t>0.00903135364021573</t>
+  </si>
+  <si>
+    <t>0.00797686150750981</t>
+  </si>
+  <si>
+    <t>0.00624662037039186</t>
+  </si>
+  <si>
+    <t>0.0127494456762749</t>
+  </si>
+  <si>
+    <t>0.00524342900945076</t>
+  </si>
+  <si>
+    <t>5.25040455520443e-06</t>
+  </si>
+  <si>
+    <t>4.33317623264638e-05</t>
+  </si>
+  <si>
+    <t>3.26487103247413e-05</t>
+  </si>
+  <si>
+    <t>0.000202052898728134</t>
+  </si>
+  <si>
+    <t>1.61903854893199e-08</t>
+  </si>
+  <si>
+    <t>6.41801990516264e-09</t>
+  </si>
+  <si>
+    <t>7.11622818759997e-08</t>
+  </si>
+  <si>
+    <t>1.55079101509388e-08</t>
+  </si>
+  <si>
+    <t>7.89576924120897e-08</t>
+  </si>
+  <si>
+    <t>1.0295953547254e-08</t>
+  </si>
+  <si>
+    <t>1.47004966375887e-05</t>
+  </si>
+  <si>
+    <t>6.68386574590285e-06</t>
+  </si>
+  <si>
+    <t>2.36534464282882e-05</t>
+  </si>
+  <si>
+    <t>4.60945311597303e-06</t>
+  </si>
+  <si>
+    <t>0.096734483266991</t>
+  </si>
+  <si>
+    <t>0.000163627132751468</t>
+  </si>
+  <si>
+    <t>0.0246395916548065</t>
+  </si>
+  <si>
+    <t>0.402270131353512</t>
+  </si>
+  <si>
+    <t>4.93964841293736e-05</t>
+  </si>
+  <si>
+    <t>0.607123472836888</t>
+  </si>
+  <si>
+    <t>0.318612649405697</t>
+  </si>
+  <si>
+    <t>0.044156696417779</t>
+  </si>
+  <si>
+    <t>0.0282918967922289</t>
+  </si>
+  <si>
+    <t>0.836114093173751</t>
+  </si>
+  <si>
+    <t>0.00945755657983383</t>
+  </si>
+  <si>
+    <t>4.10451261844451e-05</t>
+  </si>
+  <si>
+    <t>0.00104820875718709</t>
+  </si>
+  <si>
+    <t>0.011976946270974</t>
+  </si>
+  <si>
+    <t>0.00500741232165381</t>
+  </si>
+  <si>
+    <t>0.000113532255007266</t>
+  </si>
+  <si>
+    <t>0.00218674657529147</t>
+  </si>
+  <si>
+    <t>0.00569747647147028</t>
+  </si>
+  <si>
+    <t>0.0231215533088235</t>
+  </si>
+  <si>
+    <t>0.012154348670545</t>
+  </si>
+  <si>
+    <t>8.27009569708101e-05</t>
+  </si>
+  <si>
+    <t>0.0282046234542625</t>
+  </si>
+  <si>
+    <t>0.00161468096010334</t>
+  </si>
+  <si>
+    <t>0.746868131868132</t>
+  </si>
+  <si>
+    <t>0.000219001455257193</t>
+  </si>
+  <si>
+    <t>0.21750995610717</t>
+  </si>
+  <si>
+    <t>0.00822016494081365</t>
+  </si>
+  <si>
+    <t>0.893993187607115</t>
+  </si>
+  <si>
+    <t>0.000805616430639342</t>
+  </si>
+  <si>
+    <t>0.0569477219588273</t>
+  </si>
+  <si>
+    <t>0.383915784911393</t>
+  </si>
+  <si>
+    <t>1.9537432871929e-05</t>
+  </si>
+  <si>
+    <t>0.626676831093846</t>
+  </si>
+  <si>
+    <t>0.000185629380449836</t>
+  </si>
+  <si>
+    <t>2.51932885079415e-05</t>
+  </si>
+  <si>
+    <t>0.595175296839384</t>
+  </si>
+  <si>
+    <t>0.000639587697669676</t>
+  </si>
+  <si>
+    <t>0.000977558653519211</t>
+  </si>
+  <si>
+    <t>0.113969415517403</t>
+  </si>
+  <si>
+    <t>0.00114242869685098</t>
+  </si>
+  <si>
+    <t>0.0483572885956853</t>
+  </si>
+  <si>
+    <t>0.0174685548179122</t>
+  </si>
+  <si>
+    <t>0.0092456298243282</t>
+  </si>
+  <si>
+    <t>5.95828077435558e-07</t>
+  </si>
+  <si>
+    <t>9.08074202511464e-06</t>
+  </si>
+  <si>
+    <t>0.17160911258357</t>
+  </si>
+  <si>
+    <t>0.000143563367622091</t>
+  </si>
+  <si>
+    <t>0.000913437676602506</t>
+  </si>
+  <si>
+    <t>0.00553056500517969</t>
+  </si>
+  <si>
+    <t>2.86284374211232e-05</t>
+  </si>
+  <si>
+    <t>0.00387388495276873</t>
+  </si>
+  <si>
+    <t>0.000565868313504527</t>
+  </si>
+  <si>
+    <t>0.253243505648334</t>
+  </si>
+  <si>
+    <t>0.0309973045822102</t>
+  </si>
+  <si>
+    <t>0.00113236645668863</t>
+  </si>
+  <si>
+    <t>0.0303914182752755</t>
+  </si>
+  <si>
+    <t>0.00506076534503442</t>
+  </si>
+  <si>
+    <t>0.980964042311773</t>
+  </si>
+  <si>
+    <t>0.166826509672024</t>
+  </si>
+  <si>
+    <t>0.00847692505557762</t>
+  </si>
+  <si>
+    <t>0.0015066900312802</t>
+  </si>
+  <si>
+    <t>0.836079058556123</t>
+  </si>
+  <si>
+    <t>0.00360750360750361</t>
+  </si>
+  <si>
+    <t>0.983190667976553</t>
+  </si>
+  <si>
+    <t>0.00728786631870332</t>
+  </si>
+  <si>
+    <t>0.00025113995702231</t>
+  </si>
+  <si>
+    <t>0.967659936502667</t>
+  </si>
+  <si>
+    <t>0.0182515288372218</t>
+  </si>
+  <si>
+    <t>0.798259117337451</t>
+  </si>
+  <si>
+    <t>0.335964220835861</t>
+  </si>
+  <si>
+    <t>0.679749059245919</t>
+  </si>
+  <si>
+    <t>0.151843381654691</t>
+  </si>
+  <si>
+    <t>0.609976717424465</t>
+  </si>
+  <si>
+    <t>0.368222354095765</t>
+  </si>
+  <si>
+    <t>0.0100945080024578</t>
+  </si>
+  <si>
+    <t>0.273356196783349</t>
+  </si>
+  <si>
+    <t>0.00557530704589528</t>
+  </si>
+  <si>
+    <t>0.26702201453032</t>
+  </si>
+  <si>
+    <t>0.0425925925925926</t>
+  </si>
+  <si>
+    <t>0.0586111700998089</t>
+  </si>
+  <si>
+    <t>2.78149004832603e-06</t>
+  </si>
+  <si>
+    <t>3.75125148681097e-07</t>
+  </si>
+  <si>
+    <t>3.38058091660482e-05</t>
+  </si>
+  <si>
+    <t>2.2954639695184e-07</t>
+  </si>
+  <si>
+    <t>1.85041113389957e-05</t>
+  </si>
+  <si>
+    <t>0.000196506471823707</t>
+  </si>
+  <si>
+    <t>0.00013487951659564</t>
+  </si>
+  <si>
+    <t>0.000258560428190072</t>
+  </si>
+  <si>
+    <t>4.13561301936196e-05</t>
+  </si>
+  <si>
+    <t>0.000284789920765053</t>
+  </si>
+  <si>
+    <t>0.000469605871707181</t>
+  </si>
+  <si>
+    <t>0.00104782191414136</t>
+  </si>
+  <si>
+    <t>0.0050944426609144</t>
+  </si>
+  <si>
+    <t>4.88813135596899e-06</t>
+  </si>
+  <si>
+    <t>0.117057882412871</t>
+  </si>
+  <si>
+    <t>4.41189162954007e-05</t>
+  </si>
+  <si>
+    <t>9.62921705251091e-06</t>
+  </si>
+  <si>
+    <t>0.0278080052938011</t>
+  </si>
+  <si>
+    <t>0.0591093745102966</t>
+  </si>
+  <si>
+    <t>0.00200969891041731</t>
+  </si>
+  <si>
+    <t>1.74057272453244e-05</t>
+  </si>
+  <si>
+    <t>0.0724843216369528</t>
+  </si>
+  <si>
+    <t>0.0171630724683371</t>
+  </si>
+  <si>
+    <t>0.0023176521063757</t>
+  </si>
+  <si>
+    <t>4.17871242102078e-08</t>
+  </si>
+  <si>
+    <t>0.0595038687633051</t>
+  </si>
+  <si>
+    <t>0.4843285080777</t>
+  </si>
+  <si>
+    <t>1.54261883664885e-10</t>
+  </si>
+  <si>
+    <t>0.000452502515718498</t>
+  </si>
+  <si>
+    <t>0.0461538061359371</t>
+  </si>
+  <si>
+    <t>0.229367332705974</t>
+  </si>
+  <si>
+    <t>0.00105309539500406</t>
+  </si>
+  <si>
+    <t>0.000498871754172498</t>
+  </si>
+  <si>
+    <t>0.0929940074155701</t>
+  </si>
+  <si>
+    <t>0.000788205131937839</t>
+  </si>
+  <si>
+    <t>0.00153197078202238</t>
+  </si>
+  <si>
+    <t>0.238695467018003</t>
+  </si>
+  <si>
+    <t>0.223423363479975</t>
+  </si>
+  <si>
+    <t>2.14217644644319e-05</t>
+  </si>
+  <si>
+    <t>0.00129648844398106</t>
+  </si>
+  <si>
+    <t>0.154739769519383</t>
+  </si>
+  <si>
+    <t>1.65162373823297e-05</t>
+  </si>
+  <si>
+    <t>0.00486909550946644</t>
+  </si>
+  <si>
+    <t>2.36005473626224e-05</t>
+  </si>
+  <si>
+    <t>0.00319080888597653</t>
+  </si>
+  <si>
+    <t>0.00311938614382328</t>
+  </si>
+  <si>
+    <t>0.0811481617346355</t>
+  </si>
+  <si>
+    <t>0.0549944852161022</t>
+  </si>
+  <si>
+    <t>0.000467492158702212</t>
+  </si>
+  <si>
+    <t>0.595884915015473</t>
+  </si>
+  <si>
+    <t>0.944580460043499</t>
+  </si>
+  <si>
+    <t>0.000102671147849153</t>
+  </si>
+  <si>
+    <t>0.000232617674030777</t>
+  </si>
+  <si>
+    <t>0.000181609341405801</t>
+  </si>
+  <si>
+    <t>2.602627835998e-05</t>
+  </si>
+  <si>
+    <t>0.0323639896115961</t>
+  </si>
+  <si>
+    <t>0.13949125871143</t>
+  </si>
+  <si>
+    <t>1.66926251630606e-05</t>
+  </si>
+  <si>
+    <t>0.0519753339971325</t>
+  </si>
+  <si>
+    <t>0.000204825584149937</t>
+  </si>
+  <si>
+    <t>0.114451848513366</t>
+  </si>
+  <si>
+    <t>0.120880771003017</t>
+  </si>
+  <si>
+    <t>2.0135486641859e-05</t>
+  </si>
+  <si>
+    <t>0.000390029886454795</t>
+  </si>
+  <si>
+    <t>0.00821477387871993</t>
+  </si>
+  <si>
+    <t>0.407669769194311</t>
+  </si>
+  <si>
+    <t>0.000144090866428386</t>
+  </si>
+  <si>
+    <t>3.40602209501098e-05</t>
+  </si>
+  <si>
+    <t>0.00433218265413629</t>
+  </si>
+  <si>
+    <t>0.873625785256012</t>
+  </si>
+  <si>
+    <t>0.00248977029162788</t>
+  </si>
+  <si>
+    <t>0.00455205172186304</t>
+  </si>
+  <si>
+    <t>0.0608359611918331</t>
+  </si>
+  <si>
+    <t>9.61396449242447e-05</t>
+  </si>
+  <si>
+    <t>0.714080037609449</t>
+  </si>
+  <si>
+    <t>2.86280207748153e-05</t>
+  </si>
+  <si>
+    <t>0.000718031968031968</t>
+  </si>
+  <si>
+    <t>0.00354792266556972</t>
+  </si>
+  <si>
+    <t>0.611844779825852</t>
+  </si>
+  <si>
+    <t>1.82761229763763e-05</t>
+  </si>
+  <si>
+    <t>0.000535179106607678</t>
+  </si>
+  <si>
+    <t>0.384662129314536</t>
+  </si>
+  <si>
+    <t>0.00839896759321679</t>
+  </si>
+  <si>
+    <t>0.647828504216372</t>
+  </si>
+  <si>
+    <t>0.71463730223519</t>
+  </si>
+  <si>
+    <t>1.30301987887127e-05</t>
+  </si>
+  <si>
+    <t>0.0165434565434565</t>
+  </si>
+  <si>
+    <t>0.890433838607213</t>
+  </si>
+  <si>
+    <t>0.00205151990866277</t>
+  </si>
+  <si>
+    <t>0.00108151280948678</t>
+  </si>
+  <si>
+    <t>0.744491266292092</t>
+  </si>
+  <si>
+    <t>0.908910458446062</t>
+  </si>
+  <si>
+    <t>0.00793614280456386</t>
+  </si>
+  <si>
+    <t>0.0113090034965035</t>
+  </si>
+  <si>
+    <t>0.000119075970469159</t>
+  </si>
+  <si>
+    <t>0.0269582458724946</t>
   </si>
 </sst>
 </file>
@@ -7753,13 +7657,13 @@
         <v>532</v>
       </c>
       <c r="D6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F6" t="s">
-        <v>544</v>
+        <v>557</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
@@ -7839,16 +7743,16 @@
         <v>533</v>
       </c>
       <c r="D7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E7" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F7" t="s">
-        <v>555</v>
+        <v>580</v>
       </c>
       <c r="G7" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -7925,19 +7829,19 @@
         <v>534</v>
       </c>
       <c r="D8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E8" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F8" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="G8" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="H8" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="I8" t="s">
         <v>13</v>
@@ -8011,22 +7915,22 @@
         <v>535</v>
       </c>
       <c r="D9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E9" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F9" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="G9" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="H9" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="I9" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="J9" t="s">
         <v>13</v>
@@ -8094,28 +7998,28 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E10" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F10" t="s">
-        <v>588</v>
+        <v>537</v>
       </c>
       <c r="G10" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="H10" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="I10" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="J10" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="K10" t="s">
         <v>13</v>
@@ -8180,31 +8084,31 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D11" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E11" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F11" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="G11" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="H11" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="I11" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="J11" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="K11" t="s">
-        <v>675</v>
+        <v>661</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
@@ -8266,34 +8170,34 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E12" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F12" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="G12" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="H12" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="I12" t="s">
-        <v>640</v>
+        <v>561</v>
       </c>
       <c r="J12" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="K12" t="s">
-        <v>676</v>
+        <v>662</v>
       </c>
       <c r="L12" t="s">
-        <v>596</v>
+        <v>674</v>
       </c>
       <c r="M12" t="s">
         <v>13</v>
@@ -8352,37 +8256,37 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D13" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E13" t="s">
-        <v>574</v>
+        <v>552</v>
       </c>
       <c r="F13" t="s">
-        <v>541</v>
+        <v>585</v>
       </c>
       <c r="G13" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="H13" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="I13" t="s">
-        <v>641</v>
+        <v>533</v>
       </c>
       <c r="J13" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="K13" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="L13" t="s">
-        <v>691</v>
+        <v>675</v>
       </c>
       <c r="M13" t="s">
-        <v>605</v>
+        <v>685</v>
       </c>
       <c r="N13" t="s">
         <v>13</v>
@@ -8438,40 +8342,40 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D14" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E14" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F14" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="G14" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="H14" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="I14" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="J14" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="K14" t="s">
-        <v>678</v>
+        <v>664</v>
       </c>
       <c r="L14" t="s">
-        <v>692</v>
+        <v>676</v>
       </c>
       <c r="M14" t="s">
-        <v>703</v>
+        <v>686</v>
       </c>
       <c r="N14" t="s">
-        <v>538</v>
+        <v>698</v>
       </c>
       <c r="O14" t="s">
         <v>13</v>
@@ -8524,43 +8428,43 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D15" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E15" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F15" t="s">
-        <v>539</v>
+        <v>587</v>
       </c>
       <c r="G15" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="H15" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="I15" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="J15" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="K15" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="L15" t="s">
-        <v>548</v>
+        <v>677</v>
       </c>
       <c r="M15" t="s">
-        <v>704</v>
+        <v>687</v>
       </c>
       <c r="N15" t="s">
-        <v>661</v>
+        <v>699</v>
       </c>
       <c r="O15" t="s">
-        <v>691</v>
+        <v>538</v>
       </c>
       <c r="P15" t="s">
         <v>13</v>
@@ -8613,43 +8517,43 @@
         <v>541</v>
       </c>
       <c r="D16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E16" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F16" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G16" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="H16" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="I16" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="J16" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="K16" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="L16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="M16" t="s">
-        <v>705</v>
+        <v>688</v>
       </c>
       <c r="N16" t="s">
-        <v>717</v>
+        <v>700</v>
       </c>
       <c r="O16" t="s">
-        <v>726</v>
+        <v>713</v>
       </c>
       <c r="P16" t="s">
-        <v>737</v>
+        <v>721</v>
       </c>
       <c r="Q16" t="s">
         <v>13</v>
@@ -8696,49 +8600,49 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="D17" t="s">
-        <v>544</v>
+        <v>559</v>
       </c>
       <c r="E17" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="F17" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="G17" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="H17" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="I17" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="J17" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="K17" t="s">
-        <v>681</v>
+        <v>667</v>
       </c>
       <c r="L17" t="s">
-        <v>693</v>
+        <v>678</v>
       </c>
       <c r="M17" t="s">
-        <v>706</v>
+        <v>689</v>
       </c>
       <c r="N17" t="s">
-        <v>718</v>
+        <v>701</v>
       </c>
       <c r="O17" t="s">
-        <v>727</v>
+        <v>714</v>
       </c>
       <c r="P17" t="s">
-        <v>738</v>
+        <v>701</v>
       </c>
       <c r="Q17" t="s">
-        <v>747</v>
+        <v>728</v>
       </c>
       <c r="R17" t="s">
         <v>13</v>
@@ -8782,52 +8686,52 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D18" t="s">
         <v>560</v>
       </c>
       <c r="E18" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F18" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="G18" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="H18" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="I18" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="J18" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="K18" t="s">
-        <v>682</v>
+        <v>578</v>
       </c>
       <c r="L18" t="s">
-        <v>694</v>
+        <v>679</v>
       </c>
       <c r="M18" t="s">
-        <v>536</v>
+        <v>690</v>
       </c>
       <c r="N18" t="s">
-        <v>613</v>
+        <v>702</v>
       </c>
       <c r="O18" t="s">
-        <v>586</v>
+        <v>715</v>
       </c>
       <c r="P18" t="s">
-        <v>585</v>
+        <v>722</v>
       </c>
       <c r="Q18" t="s">
-        <v>748</v>
+        <v>627</v>
       </c>
       <c r="R18" t="s">
-        <v>757</v>
+        <v>717</v>
       </c>
       <c r="S18" t="s">
         <v>13</v>
@@ -8868,55 +8772,55 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D19" t="s">
         <v>561</v>
       </c>
       <c r="E19" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="F19" t="s">
-        <v>595</v>
+        <v>546</v>
       </c>
       <c r="G19" t="s">
-        <v>555</v>
+        <v>606</v>
       </c>
       <c r="H19" t="s">
-        <v>595</v>
+        <v>536</v>
       </c>
       <c r="I19" t="s">
-        <v>647</v>
+        <v>537</v>
       </c>
       <c r="J19" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="K19" t="s">
-        <v>683</v>
+        <v>668</v>
       </c>
       <c r="L19" t="s">
-        <v>695</v>
+        <v>680</v>
       </c>
       <c r="M19" t="s">
-        <v>707</v>
+        <v>616</v>
       </c>
       <c r="N19" t="s">
-        <v>560</v>
+        <v>703</v>
       </c>
       <c r="O19" t="s">
-        <v>728</v>
+        <v>627</v>
       </c>
       <c r="P19" t="s">
-        <v>739</v>
+        <v>723</v>
       </c>
       <c r="Q19" t="s">
-        <v>749</v>
+        <v>729</v>
       </c>
       <c r="R19" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="S19" t="s">
-        <v>766</v>
+        <v>744</v>
       </c>
       <c r="T19" t="s">
         <v>13</v>
@@ -8957,55 +8861,55 @@
         <v>535</v>
       </c>
       <c r="D20" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E20" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F20" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="G20" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H20" t="s">
-        <v>631</v>
+        <v>616</v>
       </c>
       <c r="I20" t="s">
+        <v>641</v>
+      </c>
+      <c r="J20" t="s">
+        <v>136</v>
+      </c>
+      <c r="K20" t="s">
+        <v>647</v>
+      </c>
+      <c r="L20" t="s">
         <v>648</v>
       </c>
-      <c r="J20" t="s">
-        <v>666</v>
-      </c>
-      <c r="K20" t="s">
-        <v>656</v>
-      </c>
-      <c r="L20" t="s">
-        <v>696</v>
-      </c>
       <c r="M20" t="s">
-        <v>708</v>
+        <v>691</v>
       </c>
       <c r="N20" t="s">
-        <v>677</v>
+        <v>704</v>
       </c>
       <c r="O20" t="s">
-        <v>729</v>
+        <v>716</v>
       </c>
       <c r="P20" t="s">
-        <v>622</v>
+        <v>724</v>
       </c>
       <c r="Q20" t="s">
-        <v>750</v>
+        <v>730</v>
       </c>
       <c r="R20" t="s">
-        <v>758</v>
+        <v>738</v>
       </c>
       <c r="S20" t="s">
-        <v>767</v>
+        <v>745</v>
       </c>
       <c r="T20" t="s">
-        <v>773</v>
+        <v>752</v>
       </c>
       <c r="U20" t="s">
         <v>13</v>
@@ -9043,58 +8947,58 @@
         <v>533</v>
       </c>
       <c r="D21" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E21" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F21" t="s">
-        <v>555</v>
+        <v>580</v>
       </c>
       <c r="G21" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="H21" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="I21" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="J21" t="s">
-        <v>667</v>
+        <v>627</v>
       </c>
       <c r="K21" t="s">
-        <v>684</v>
+        <v>669</v>
       </c>
       <c r="L21" t="s">
-        <v>697</v>
+        <v>681</v>
       </c>
       <c r="M21" t="s">
-        <v>709</v>
+        <v>692</v>
       </c>
       <c r="N21" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
       <c r="O21" t="s">
-        <v>730</v>
+        <v>599</v>
       </c>
       <c r="P21" t="s">
-        <v>619</v>
+        <v>725</v>
       </c>
       <c r="Q21" t="s">
-        <v>562</v>
+        <v>656</v>
       </c>
       <c r="R21" t="s">
-        <v>759</v>
+        <v>739</v>
       </c>
       <c r="S21" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="T21" t="s">
-        <v>595</v>
+        <v>753</v>
       </c>
       <c r="U21" t="s">
-        <v>779</v>
+        <v>627</v>
       </c>
       <c r="V21" t="s">
         <v>13</v>
@@ -9126,64 +9030,64 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D22" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E22" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F22" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="G22" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="H22" t="s">
-        <v>552</v>
+        <v>627</v>
       </c>
       <c r="I22" t="s">
-        <v>613</v>
+        <v>641</v>
       </c>
       <c r="J22" t="s">
-        <v>668</v>
+        <v>656</v>
       </c>
       <c r="K22" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="L22" t="s">
-        <v>698</v>
+        <v>648</v>
       </c>
       <c r="M22" t="s">
-        <v>710</v>
+        <v>537</v>
       </c>
       <c r="N22" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="O22" t="s">
+        <v>640</v>
+      </c>
+      <c r="P22" t="s">
+        <v>726</v>
+      </c>
+      <c r="Q22" t="s">
         <v>731</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>740</v>
       </c>
-      <c r="Q22" t="s">
-        <v>751</v>
-      </c>
-      <c r="R22" t="s">
-        <v>760</v>
-      </c>
       <c r="S22" t="s">
-        <v>682</v>
+        <v>746</v>
       </c>
       <c r="T22" t="s">
-        <v>774</v>
+        <v>754</v>
       </c>
       <c r="U22" t="s">
-        <v>668</v>
+        <v>656</v>
       </c>
       <c r="V22" t="s">
-        <v>552</v>
+        <v>627</v>
       </c>
       <c r="W22" t="s">
         <v>13</v>
@@ -9215,64 +9119,64 @@
         <v>533</v>
       </c>
       <c r="D23" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E23" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F23" t="s">
-        <v>555</v>
+        <v>580</v>
       </c>
       <c r="G23" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="H23" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="I23" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="J23" t="s">
-        <v>669</v>
+        <v>657</v>
       </c>
       <c r="K23" t="s">
-        <v>686</v>
+        <v>670</v>
       </c>
       <c r="L23" t="s">
-        <v>699</v>
+        <v>682</v>
       </c>
       <c r="M23" t="s">
-        <v>711</v>
+        <v>693</v>
       </c>
       <c r="N23" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
       <c r="O23" t="s">
+        <v>564</v>
+      </c>
+      <c r="P23" t="s">
+        <v>621</v>
+      </c>
+      <c r="Q23" t="s">
         <v>732</v>
       </c>
-      <c r="P23" t="s">
-        <v>741</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>679</v>
-      </c>
       <c r="R23" t="s">
-        <v>761</v>
+        <v>727</v>
       </c>
       <c r="S23" t="s">
-        <v>768</v>
+        <v>747</v>
       </c>
       <c r="T23" t="s">
-        <v>775</v>
+        <v>755</v>
       </c>
       <c r="U23" t="s">
-        <v>754</v>
+        <v>136</v>
       </c>
       <c r="V23" t="s">
-        <v>533</v>
+        <v>557</v>
       </c>
       <c r="W23" t="s">
-        <v>552</v>
+        <v>627</v>
       </c>
       <c r="X23" t="s">
         <v>13</v>
@@ -9298,70 +9202,70 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D24" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E24" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="F24" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="G24" t="s">
-        <v>586</v>
+        <v>605</v>
       </c>
       <c r="H24" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
       <c r="I24" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
       <c r="J24" t="s">
-        <v>670</v>
+        <v>658</v>
       </c>
       <c r="K24" t="s">
-        <v>687</v>
+        <v>578</v>
       </c>
       <c r="L24" t="s">
-        <v>700</v>
+        <v>679</v>
       </c>
       <c r="M24" t="s">
-        <v>712</v>
+        <v>694</v>
       </c>
       <c r="N24" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="O24" t="s">
+        <v>717</v>
+      </c>
+      <c r="P24" t="s">
+        <v>709</v>
+      </c>
+      <c r="Q24" t="s">
         <v>733</v>
       </c>
-      <c r="P24" t="s">
-        <v>742</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>752</v>
-      </c>
       <c r="R24" t="s">
-        <v>560</v>
+        <v>741</v>
       </c>
       <c r="S24" t="s">
-        <v>136</v>
+        <v>748</v>
       </c>
       <c r="T24" t="s">
-        <v>776</v>
+        <v>756</v>
       </c>
       <c r="U24" t="s">
-        <v>780</v>
+        <v>760</v>
       </c>
       <c r="V24" t="s">
-        <v>784</v>
+        <v>625</v>
       </c>
       <c r="W24" t="s">
-        <v>787</v>
+        <v>745</v>
       </c>
       <c r="X24" t="s">
-        <v>789</v>
+        <v>763</v>
       </c>
       <c r="Y24" t="s">
         <v>13</v>
@@ -9387,70 +9291,70 @@
         <v>545</v>
       </c>
       <c r="D25" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E25" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="F25" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="G25" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="H25" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="I25" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="J25" t="s">
+        <v>659</v>
+      </c>
+      <c r="K25" t="s">
         <v>671</v>
       </c>
-      <c r="K25" t="s">
-        <v>688</v>
-      </c>
       <c r="L25" t="s">
-        <v>701</v>
+        <v>683</v>
       </c>
       <c r="M25" t="s">
-        <v>713</v>
+        <v>695</v>
       </c>
       <c r="N25" t="s">
-        <v>689</v>
+        <v>709</v>
       </c>
       <c r="O25" t="s">
-        <v>702</v>
+        <v>626</v>
       </c>
       <c r="P25" t="s">
-        <v>743</v>
+        <v>727</v>
       </c>
       <c r="Q25" t="s">
-        <v>753</v>
+        <v>620</v>
       </c>
       <c r="R25" t="s">
-        <v>762</v>
+        <v>624</v>
       </c>
       <c r="S25" t="s">
-        <v>769</v>
+        <v>749</v>
       </c>
       <c r="T25" t="s">
-        <v>777</v>
+        <v>731</v>
       </c>
       <c r="U25" t="s">
-        <v>781</v>
+        <v>659</v>
       </c>
       <c r="V25" t="s">
-        <v>535</v>
+        <v>761</v>
       </c>
       <c r="W25" t="s">
-        <v>702</v>
+        <v>659</v>
       </c>
       <c r="X25" t="s">
-        <v>790</v>
+        <v>557</v>
       </c>
       <c r="Y25" t="s">
-        <v>793</v>
+        <v>749</v>
       </c>
       <c r="Z25" t="s">
         <v>13</v>
@@ -9473,73 +9377,73 @@
         <v>546</v>
       </c>
       <c r="D26" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E26" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="F26" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="G26" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="H26" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="I26" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="J26" t="s">
+        <v>660</v>
+      </c>
+      <c r="K26" t="s">
         <v>672</v>
       </c>
-      <c r="K26" t="s">
-        <v>689</v>
-      </c>
       <c r="L26" t="s">
-        <v>702</v>
+        <v>550</v>
       </c>
       <c r="M26" t="s">
-        <v>714</v>
+        <v>696</v>
       </c>
       <c r="N26" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
       <c r="O26" t="s">
+        <v>718</v>
+      </c>
+      <c r="P26" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q26" t="s">
         <v>734</v>
       </c>
-      <c r="P26" t="s">
-        <v>744</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>754</v>
-      </c>
       <c r="R26" t="s">
-        <v>763</v>
+        <v>742</v>
       </c>
       <c r="S26" t="s">
-        <v>770</v>
+        <v>750</v>
       </c>
       <c r="T26" t="s">
-        <v>605</v>
+        <v>757</v>
       </c>
       <c r="U26" t="s">
-        <v>782</v>
+        <v>136</v>
       </c>
       <c r="V26" t="s">
-        <v>785</v>
+        <v>640</v>
       </c>
       <c r="W26" t="s">
-        <v>635</v>
+        <v>762</v>
       </c>
       <c r="X26" t="s">
-        <v>791</v>
+        <v>764</v>
       </c>
       <c r="Y26" t="s">
-        <v>794</v>
+        <v>766</v>
       </c>
       <c r="Z26" t="s">
-        <v>797</v>
+        <v>768</v>
       </c>
       <c r="AA26" t="s">
         <v>13</v>
@@ -9556,79 +9460,79 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D27" t="s">
+        <v>563</v>
+      </c>
+      <c r="E27" t="s">
+        <v>578</v>
+      </c>
+      <c r="F27" t="s">
+        <v>592</v>
+      </c>
+      <c r="G27" t="s">
+        <v>613</v>
+      </c>
+      <c r="H27" t="s">
+        <v>631</v>
+      </c>
+      <c r="I27" t="s">
+        <v>645</v>
+      </c>
+      <c r="J27" t="s">
+        <v>660</v>
+      </c>
+      <c r="K27" t="s">
+        <v>672</v>
+      </c>
+      <c r="L27" t="s">
+        <v>550</v>
+      </c>
+      <c r="M27" t="s">
+        <v>696</v>
+      </c>
+      <c r="N27" t="s">
+        <v>711</v>
+      </c>
+      <c r="O27" t="s">
+        <v>719</v>
+      </c>
+      <c r="P27" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>735</v>
+      </c>
+      <c r="R27" t="s">
         <v>565</v>
       </c>
-      <c r="E27" t="s">
-        <v>584</v>
-      </c>
-      <c r="F27" t="s">
-        <v>599</v>
-      </c>
-      <c r="G27" t="s">
-        <v>619</v>
-      </c>
-      <c r="H27" t="s">
-        <v>576</v>
-      </c>
-      <c r="I27" t="s">
-        <v>654</v>
-      </c>
-      <c r="J27" t="s">
-        <v>673</v>
-      </c>
-      <c r="K27" t="s">
-        <v>690</v>
-      </c>
-      <c r="L27" t="s">
-        <v>585</v>
-      </c>
-      <c r="M27" t="s">
-        <v>715</v>
-      </c>
-      <c r="N27" t="s">
-        <v>724</v>
-      </c>
-      <c r="O27" t="s">
-        <v>735</v>
-      </c>
-      <c r="P27" t="s">
-        <v>745</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>755</v>
-      </c>
-      <c r="R27" t="s">
-        <v>764</v>
-      </c>
       <c r="S27" t="s">
-        <v>771</v>
+        <v>751</v>
       </c>
       <c r="T27" t="s">
-        <v>778</v>
+        <v>758</v>
       </c>
       <c r="U27" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
       <c r="V27" t="s">
-        <v>576</v>
+        <v>640</v>
       </c>
       <c r="W27" t="s">
-        <v>690</v>
+        <v>762</v>
       </c>
       <c r="X27" t="s">
-        <v>576</v>
+        <v>765</v>
       </c>
       <c r="Y27" t="s">
-        <v>795</v>
+        <v>767</v>
       </c>
       <c r="Z27" t="s">
-        <v>613</v>
+        <v>768</v>
       </c>
       <c r="AA27" t="s">
-        <v>799</v>
+        <v>136</v>
       </c>
       <c r="AB27" t="s">
         <v>13</v>
@@ -9642,82 +9546,82 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D28" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E28" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="F28" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="G28" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="H28" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="I28" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="J28" t="s">
-        <v>674</v>
+        <v>640</v>
       </c>
       <c r="K28" t="s">
-        <v>624</v>
+        <v>673</v>
       </c>
       <c r="L28" t="s">
-        <v>563</v>
+        <v>684</v>
       </c>
       <c r="M28" t="s">
-        <v>716</v>
+        <v>697</v>
       </c>
       <c r="N28" t="s">
-        <v>725</v>
+        <v>712</v>
       </c>
       <c r="O28" t="s">
+        <v>720</v>
+      </c>
+      <c r="P28" t="s">
+        <v>593</v>
+      </c>
+      <c r="Q28" t="s">
         <v>736</v>
       </c>
-      <c r="P28" t="s">
-        <v>746</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>756</v>
-      </c>
       <c r="R28" t="s">
-        <v>765</v>
+        <v>743</v>
       </c>
       <c r="S28" t="s">
-        <v>772</v>
+        <v>590</v>
       </c>
       <c r="T28" t="s">
-        <v>616</v>
+        <v>759</v>
       </c>
       <c r="U28" t="s">
-        <v>783</v>
+        <v>640</v>
       </c>
       <c r="V28" t="s">
-        <v>786</v>
+        <v>699</v>
       </c>
       <c r="W28" t="s">
-        <v>788</v>
+        <v>640</v>
       </c>
       <c r="X28" t="s">
-        <v>792</v>
+        <v>533</v>
       </c>
       <c r="Y28" t="s">
-        <v>796</v>
+        <v>590</v>
       </c>
       <c r="Z28" t="s">
-        <v>798</v>
+        <v>769</v>
       </c>
       <c r="AA28" t="s">
-        <v>800</v>
+        <v>537</v>
       </c>
       <c r="AB28" t="s">
-        <v>801</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new stat results with phi f,d
</commit_message>
<xml_diff>
--- a/02_pam/output/stat_results/pairwise_allmetsxtissues.xlsx
+++ b/02_pam/output/stat_results/pairwise_allmetsxtissues.xlsx
@@ -9,12 +9,13 @@
     <sheet name="Fv.Fm" r:id="rId3" sheetId="1"/>
     <sheet name="φPSII" r:id="rId4" sheetId="2"/>
     <sheet name="ΦNPQ" r:id="rId5" sheetId="3"/>
+    <sheet name="Φf.D" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3124" uniqueCount="1017">
   <si>
     <t/>
   </si>
@@ -2324,6 +2325,747 @@
   </si>
   <si>
     <t>0.0269582458724946</t>
+  </si>
+  <si>
+    <t>1.46914413092828e-06</t>
+  </si>
+  <si>
+    <t>1.97325911664838e-06</t>
+  </si>
+  <si>
+    <t>1.37582108242688e-05</t>
+  </si>
+  <si>
+    <t>1.89780302773899e-05</t>
+  </si>
+  <si>
+    <t>0.000102924586269731</t>
+  </si>
+  <si>
+    <t>4.84504487856965e-10</t>
+  </si>
+  <si>
+    <t>4.27413716681936e-09</t>
+  </si>
+  <si>
+    <t>6.85417095264142e-09</t>
+  </si>
+  <si>
+    <t>6.66841770080943e-06</t>
+  </si>
+  <si>
+    <t>2.98707480394053e-06</t>
+  </si>
+  <si>
+    <t>3.91284878298995e-06</t>
+  </si>
+  <si>
+    <t>2.39181431914157e-06</t>
+  </si>
+  <si>
+    <t>1.62974558250254e-06</t>
+  </si>
+  <si>
+    <t>6.47760868396346e-05</t>
+  </si>
+  <si>
+    <t>8.8306053652654e-05</t>
+  </si>
+  <si>
+    <t>0.000550670992849549</t>
+  </si>
+  <si>
+    <t>0.00077123100333586</t>
+  </si>
+  <si>
+    <t>0.00223525342731377</t>
+  </si>
+  <si>
+    <t>1.59711047350042e-06</t>
+  </si>
+  <si>
+    <t>1.52781452914049e-06</t>
+  </si>
+  <si>
+    <t>1.59002101370314e-06</t>
+  </si>
+  <si>
+    <t>4.11268967627329e-06</t>
+  </si>
+  <si>
+    <t>0.000298172236159297</t>
+  </si>
+  <si>
+    <t>0.000137871385547842</t>
+  </si>
+  <si>
+    <t>0.000177368594616916</t>
+  </si>
+  <si>
+    <t>0.000108960165287834</t>
+  </si>
+  <si>
+    <t>7.60220907448281e-05</t>
+  </si>
+  <si>
+    <t>0.00517725139988128</t>
+  </si>
+  <si>
+    <t>0.00600173139632833</t>
+  </si>
+  <si>
+    <t>0.0172760588303928</t>
+  </si>
+  <si>
+    <t>0.0225198353259596</t>
+  </si>
+  <si>
+    <t>0.0432006010518407</t>
+  </si>
+  <si>
+    <t>0.00133843987321872</t>
+  </si>
+  <si>
+    <t>0.00132102267310655</t>
+  </si>
+  <si>
+    <t>0.00133443791013325</t>
+  </si>
+  <si>
+    <t>0.0016770568502043</t>
+  </si>
+  <si>
+    <t>0.00183777596266874</t>
+  </si>
+  <si>
+    <t>0.00131826197442768</t>
+  </si>
+  <si>
+    <t>0.0113964152253623</t>
+  </si>
+  <si>
+    <t>0.00737904307983945</t>
+  </si>
+  <si>
+    <t>0.00830318766008975</t>
+  </si>
+  <si>
+    <t>0.00665913303636113</t>
+  </si>
+  <si>
+    <t>0.00557432501490154</t>
+  </si>
+  <si>
+    <t>4.64475228235315e-06</t>
+  </si>
+  <si>
+    <t>5.00452061270906e-05</t>
+  </si>
+  <si>
+    <t>7.09662241449245e-05</t>
+  </si>
+  <si>
+    <t>0.000319870256601466</t>
+  </si>
+  <si>
+    <t>4.10307004148575e-08</t>
+  </si>
+  <si>
+    <t>8.181227864492e-08</t>
+  </si>
+  <si>
+    <t>6.8431245413214e-09</t>
+  </si>
+  <si>
+    <t>2.58926676774888e-05</t>
+  </si>
+  <si>
+    <t>1.15693532316023e-05</t>
+  </si>
+  <si>
+    <t>1.49691494917964e-05</t>
+  </si>
+  <si>
+    <t>8.57887930232797e-06</t>
+  </si>
+  <si>
+    <t>5.55167945084225e-06</t>
+  </si>
+  <si>
+    <t>0.000965878342183555</t>
+  </si>
+  <si>
+    <t>0.0147743541861189</t>
+  </si>
+  <si>
+    <t>0.000593395252837977</t>
+  </si>
+  <si>
+    <t>0.00107240105934574</t>
+  </si>
+  <si>
+    <t>0.52747462724168</t>
+  </si>
+  <si>
+    <t>0.00427981982827575</t>
+  </si>
+  <si>
+    <t>3.45421735272256e-06</t>
+  </si>
+  <si>
+    <t>0.00262153063538664</t>
+  </si>
+  <si>
+    <t>7.33593486161674e-05</t>
+  </si>
+  <si>
+    <t>8.42421556876668e-07</t>
+  </si>
+  <si>
+    <t>2.51535316335364e-06</t>
+  </si>
+  <si>
+    <t>1.8516598278697e-05</t>
+  </si>
+  <si>
+    <t>2.35018362768078e-06</t>
+  </si>
+  <si>
+    <t>0.228276520946051</t>
+  </si>
+  <si>
+    <t>0.000106853887065662</t>
+  </si>
+  <si>
+    <t>2.234446410143e-05</t>
+  </si>
+  <si>
+    <t>1.47007370949579e-06</t>
+  </si>
+  <si>
+    <t>5.2332238542903e-07</t>
+  </si>
+  <si>
+    <t>0.41235784569169</t>
+  </si>
+  <si>
+    <t>0.255118170322243</t>
+  </si>
+  <si>
+    <t>0.388475000884946</t>
+  </si>
+  <si>
+    <t>0.12278132410577</t>
+  </si>
+  <si>
+    <t>0.640435177013749</t>
+  </si>
+  <si>
+    <t>0.222615143447838</t>
+  </si>
+  <si>
+    <t>0.25369823416405</t>
+  </si>
+  <si>
+    <t>0.537341519813543</t>
+  </si>
+  <si>
+    <t>0.0045654971008991</t>
+  </si>
+  <si>
+    <t>0.110588172516772</t>
+  </si>
+  <si>
+    <t>0.074108019872502</t>
+  </si>
+  <si>
+    <t>5.02593381850348e-06</t>
+  </si>
+  <si>
+    <t>0.219983213873785</t>
+  </si>
+  <si>
+    <t>0.0040934555640438</t>
+  </si>
+  <si>
+    <t>0.000197141280012617</t>
+  </si>
+  <si>
+    <t>0.108231536802965</t>
+  </si>
+  <si>
+    <t>0.0221623928817677</t>
+  </si>
+  <si>
+    <t>0.63199813569665</t>
+  </si>
+  <si>
+    <t>3.76758890690779e-05</t>
+  </si>
+  <si>
+    <t>2.99128041758275e-06</t>
+  </si>
+  <si>
+    <t>0.974917263444279</t>
+  </si>
+  <si>
+    <t>0.882215838142486</t>
+  </si>
+  <si>
+    <t>0.034830859675753</t>
+  </si>
+  <si>
+    <t>0.109778968979575</t>
+  </si>
+  <si>
+    <t>0.653001970257221</t>
+  </si>
+  <si>
+    <t>0.109525839900054</t>
+  </si>
+  <si>
+    <t>0.864218292792991</t>
+  </si>
+  <si>
+    <t>0.890596921556674</t>
+  </si>
+  <si>
+    <t>5.35928657177157e-05</t>
+  </si>
+  <si>
+    <t>0.0547114833854163</t>
+  </si>
+  <si>
+    <t>0.00548516620270399</t>
+  </si>
+  <si>
+    <t>0.500991631476399</t>
+  </si>
+  <si>
+    <t>0.334101627628805</t>
+  </si>
+  <si>
+    <t>0.000186896142626135</t>
+  </si>
+  <si>
+    <t>0.950011526934604</t>
+  </si>
+  <si>
+    <t>0.0409350408715385</t>
+  </si>
+  <si>
+    <t>0.2260744260024</t>
+  </si>
+  <si>
+    <t>0.77746080472901</t>
+  </si>
+  <si>
+    <t>0.0417671141674737</t>
+  </si>
+  <si>
+    <t>0.578977984401115</t>
+  </si>
+  <si>
+    <t>0.311955015353317</t>
+  </si>
+  <si>
+    <t>0.911188557904474</t>
+  </si>
+  <si>
+    <t>0.544503727783471</t>
+  </si>
+  <si>
+    <t>0.000719394457534875</t>
+  </si>
+  <si>
+    <t>0.000669242766358621</t>
+  </si>
+  <si>
+    <t>0.00694654183026276</t>
+  </si>
+  <si>
+    <t>0.866582441531232</t>
+  </si>
+  <si>
+    <t>0.417214364582786</t>
+  </si>
+  <si>
+    <t>0.00362156696998326</t>
+  </si>
+  <si>
+    <t>0.0881992023724307</t>
+  </si>
+  <si>
+    <t>0.00243143100285957</t>
+  </si>
+  <si>
+    <t>0.000496472052199606</t>
+  </si>
+  <si>
+    <t>0.0516966014153839</t>
+  </si>
+  <si>
+    <t>0.351062497502936</t>
+  </si>
+  <si>
+    <t>0.981920658565482</t>
+  </si>
+  <si>
+    <t>0.0848304556751086</t>
+  </si>
+  <si>
+    <t>0.7375055285272</t>
+  </si>
+  <si>
+    <t>0.230206278613672</t>
+  </si>
+  <si>
+    <t>0.85878008001157</t>
+  </si>
+  <si>
+    <t>0.407459207459207</t>
+  </si>
+  <si>
+    <t>0.000969122901638239</t>
+  </si>
+  <si>
+    <t>0.00177971741182661</t>
+  </si>
+  <si>
+    <t>0.252584295137487</t>
+  </si>
+  <si>
+    <t>0.0722664432341852</t>
+  </si>
+  <si>
+    <t>0.00279234654234654</t>
+  </si>
+  <si>
+    <t>0.00134100622110277</t>
+  </si>
+  <si>
+    <t>0.0996880698288051</t>
+  </si>
+  <si>
+    <t>0.00174043475952857</t>
+  </si>
+  <si>
+    <t>0.0117911941505956</t>
+  </si>
+  <si>
+    <t>8.03429624641099e-05</t>
+  </si>
+  <si>
+    <t>0.000836085352458897</t>
+  </si>
+  <si>
+    <t>8.36615342040886e-05</t>
+  </si>
+  <si>
+    <t>0.0262486400669766</t>
+  </si>
+  <si>
+    <t>0.830142079839557</t>
+  </si>
+  <si>
+    <t>0.00122051474373625</t>
+  </si>
+  <si>
+    <t>0.00818806614326521</t>
+  </si>
+  <si>
+    <t>0.00212395364263973</t>
+  </si>
+  <si>
+    <t>5.83597508868402e-05</t>
+  </si>
+  <si>
+    <t>0.435133539653415</t>
+  </si>
+  <si>
+    <t>0.000363574791533674</t>
+  </si>
+  <si>
+    <t>4.17275545299923e-05</t>
+  </si>
+  <si>
+    <t>0.000459598735533525</t>
+  </si>
+  <si>
+    <t>0.138777614747971</t>
+  </si>
+  <si>
+    <t>8.6069514601272e-05</t>
+  </si>
+  <si>
+    <t>0.0942214438995076</t>
+  </si>
+  <si>
+    <t>3.21798807942617e-06</t>
+  </si>
+  <si>
+    <t>0.141236795572487</t>
+  </si>
+  <si>
+    <t>0.00124685894135588</t>
+  </si>
+  <si>
+    <t>0.0828422289728547</t>
+  </si>
+  <si>
+    <t>0.024109968720655</t>
+  </si>
+  <si>
+    <t>0.95643846763465</t>
+  </si>
+  <si>
+    <t>3.59798854605734e-05</t>
+  </si>
+  <si>
+    <t>4.88419660941623e-07</t>
+  </si>
+  <si>
+    <t>0.249374085071198</t>
+  </si>
+  <si>
+    <t>0.000724345474603722</t>
+  </si>
+  <si>
+    <t>0.450068987877592</t>
+  </si>
+  <si>
+    <t>7.17444463607316e-06</t>
+  </si>
+  <si>
+    <t>0.71934741622644</t>
+  </si>
+  <si>
+    <t>0.745878483582455</t>
+  </si>
+  <si>
+    <t>0.156722031545248</t>
+  </si>
+  <si>
+    <t>0.147698585718734</t>
+  </si>
+  <si>
+    <t>5.88473289567701e-05</t>
+  </si>
+  <si>
+    <t>0.00316811062959207</t>
+  </si>
+  <si>
+    <t>7.45115564620668e-10</t>
+  </si>
+  <si>
+    <t>1.0376690000045e-08</t>
+  </si>
+  <si>
+    <t>0.00476209352547718</t>
+  </si>
+  <si>
+    <t>0.0656128394634793</t>
+  </si>
+  <si>
+    <t>0.000230231294633637</t>
+  </si>
+  <si>
+    <t>0.00448562766171116</t>
+  </si>
+  <si>
+    <t>0.00104441013531923</t>
+  </si>
+  <si>
+    <t>0.666824197433516</t>
+  </si>
+  <si>
+    <t>1.8033773890489e-05</t>
+  </si>
+  <si>
+    <t>8.36382575950447e-08</t>
+  </si>
+  <si>
+    <t>0.0777192882398123</t>
+  </si>
+  <si>
+    <t>0.199594619511259</t>
+  </si>
+  <si>
+    <t>0.558104168502009</t>
+  </si>
+  <si>
+    <t>0.0032490636913743</t>
+  </si>
+  <si>
+    <t>0.000406129779755323</t>
+  </si>
+  <si>
+    <t>0.0606599056262665</t>
+  </si>
+  <si>
+    <t>0.306165580092081</t>
+  </si>
+  <si>
+    <t>2.8813221974895e-05</t>
+  </si>
+  <si>
+    <t>1.08163834329771e-06</t>
+  </si>
+  <si>
+    <t>0.00375000514523381</t>
+  </si>
+  <si>
+    <t>0.384601566106412</t>
+  </si>
+  <si>
+    <t>0.00219649485233478</t>
+  </si>
+  <si>
+    <t>0.376112227389182</t>
+  </si>
+  <si>
+    <t>2.44964602326803e-06</t>
+  </si>
+  <si>
+    <t>0.0775251638891432</t>
+  </si>
+  <si>
+    <t>0.123343827541559</t>
+  </si>
+  <si>
+    <t>0.543179232716163</t>
+  </si>
+  <si>
+    <t>0.0328143114148778</t>
+  </si>
+  <si>
+    <t>0.0108845806136957</t>
+  </si>
+  <si>
+    <t>0.00135531591429068</t>
+  </si>
+  <si>
+    <t>0.670219962050164</t>
+  </si>
+  <si>
+    <t>7.87148294906324e-06</t>
+  </si>
+  <si>
+    <t>0.936014987115839</t>
+  </si>
+  <si>
+    <t>0.280338586097211</t>
+  </si>
+  <si>
+    <t>4.08078070189144e-05</t>
+  </si>
+  <si>
+    <t>0.0673417303503099</t>
+  </si>
+  <si>
+    <t>6.43818589541128e-05</t>
+  </si>
+  <si>
+    <t>8.22446642880079e-05</t>
+  </si>
+  <si>
+    <t>0.335999616821535</t>
+  </si>
+  <si>
+    <t>0.627137568314039</t>
+  </si>
+  <si>
+    <t>5.53282287028417e-05</t>
+  </si>
+  <si>
+    <t>0.000385705421676645</t>
+  </si>
+  <si>
+    <t>0.00019918162333023</t>
+  </si>
+  <si>
+    <t>0.22442120419398</t>
+  </si>
+  <si>
+    <t>2.38886977793067e-05</t>
+  </si>
+  <si>
+    <t>4.20698513178289e-05</t>
+  </si>
+  <si>
+    <t>0.106360192433123</t>
+  </si>
+  <si>
+    <t>0.000398236217563949</t>
+  </si>
+  <si>
+    <t>0.285548602772797</t>
+  </si>
+  <si>
+    <t>0.771457489878543</t>
+  </si>
+  <si>
+    <t>0.555982008187891</t>
+  </si>
+  <si>
+    <t>0.30476467976468</t>
+  </si>
+  <si>
+    <t>0.00223320794078809</t>
+  </si>
+  <si>
+    <t>1.75070028011205e-05</t>
+  </si>
+  <si>
+    <t>2.83817439162549e-05</t>
+  </si>
+  <si>
+    <t>0.00750045349209293</t>
+  </si>
+  <si>
+    <t>0.791568568147089</t>
+  </si>
+  <si>
+    <t>0.00379062561803679</t>
+  </si>
+  <si>
+    <t>0.223232714138287</t>
+  </si>
+  <si>
+    <t>0.280330717026171</t>
+  </si>
+  <si>
+    <t>0.000360282414925248</t>
+  </si>
+  <si>
+    <t>0.0411794314730957</t>
+  </si>
+  <si>
+    <t>1.47427392009435e-05</t>
+  </si>
+  <si>
+    <t>0.00750969214271967</t>
+  </si>
+  <si>
+    <t>0.000238917351216816</t>
+  </si>
+  <si>
+    <t>0.000130840425853603</t>
+  </si>
+  <si>
+    <t>0.000279464012325578</t>
+  </si>
+  <si>
+    <t>0.0367477488612418</t>
+  </si>
+  <si>
+    <t>0.18500171998624</t>
+  </si>
+  <si>
+    <t>0.000144730549472677</t>
+  </si>
+  <si>
+    <t>0.142107757928539</t>
   </si>
 </sst>
 </file>
@@ -9627,4 +10369,2425 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W4" t="s">
+        <v>13</v>
+      </c>
+      <c r="X4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5" t="s">
+        <v>13</v>
+      </c>
+      <c r="U5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V5" t="s">
+        <v>13</v>
+      </c>
+      <c r="W5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>770</v>
+      </c>
+      <c r="D6" t="s">
+        <v>783</v>
+      </c>
+      <c r="E6" t="s">
+        <v>797</v>
+      </c>
+      <c r="F6" t="s">
+        <v>813</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V6" t="s">
+        <v>13</v>
+      </c>
+      <c r="W6" t="s">
+        <v>13</v>
+      </c>
+      <c r="X6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>771</v>
+      </c>
+      <c r="D7" t="s">
+        <v>784</v>
+      </c>
+      <c r="E7" t="s">
+        <v>798</v>
+      </c>
+      <c r="F7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G7" t="s">
+        <v>825</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>771</v>
+      </c>
+      <c r="D8" t="s">
+        <v>784</v>
+      </c>
+      <c r="E8" t="s">
+        <v>798</v>
+      </c>
+      <c r="F8" t="s">
+        <v>778</v>
+      </c>
+      <c r="G8" t="s">
+        <v>826</v>
+      </c>
+      <c r="H8" t="s">
+        <v>843</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8" t="s">
+        <v>13</v>
+      </c>
+      <c r="S8" t="s">
+        <v>13</v>
+      </c>
+      <c r="T8" t="s">
+        <v>13</v>
+      </c>
+      <c r="U8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>772</v>
+      </c>
+      <c r="D9" t="s">
+        <v>785</v>
+      </c>
+      <c r="E9" t="s">
+        <v>799</v>
+      </c>
+      <c r="F9" t="s">
+        <v>814</v>
+      </c>
+      <c r="G9" t="s">
+        <v>827</v>
+      </c>
+      <c r="H9" t="s">
+        <v>844</v>
+      </c>
+      <c r="I9" t="s">
+        <v>863</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" t="s">
+        <v>13</v>
+      </c>
+      <c r="S9" t="s">
+        <v>13</v>
+      </c>
+      <c r="T9" t="s">
+        <v>13</v>
+      </c>
+      <c r="U9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>773</v>
+      </c>
+      <c r="D10" t="s">
+        <v>786</v>
+      </c>
+      <c r="E10" t="s">
+        <v>800</v>
+      </c>
+      <c r="F10" t="s">
+        <v>815</v>
+      </c>
+      <c r="G10" t="s">
+        <v>828</v>
+      </c>
+      <c r="H10" t="s">
+        <v>845</v>
+      </c>
+      <c r="I10" t="s">
+        <v>864</v>
+      </c>
+      <c r="J10" t="s">
+        <v>877</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10" t="s">
+        <v>13</v>
+      </c>
+      <c r="U10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V10" t="s">
+        <v>13</v>
+      </c>
+      <c r="W10" t="s">
+        <v>13</v>
+      </c>
+      <c r="X10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>774</v>
+      </c>
+      <c r="D11" t="s">
+        <v>787</v>
+      </c>
+      <c r="E11" t="s">
+        <v>801</v>
+      </c>
+      <c r="F11" t="s">
+        <v>816</v>
+      </c>
+      <c r="G11" t="s">
+        <v>829</v>
+      </c>
+      <c r="H11" t="s">
+        <v>846</v>
+      </c>
+      <c r="I11" t="s">
+        <v>865</v>
+      </c>
+      <c r="J11" t="s">
+        <v>878</v>
+      </c>
+      <c r="K11" t="s">
+        <v>895</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>13</v>
+      </c>
+      <c r="R11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S11" t="s">
+        <v>13</v>
+      </c>
+      <c r="T11" t="s">
+        <v>13</v>
+      </c>
+      <c r="U11" t="s">
+        <v>13</v>
+      </c>
+      <c r="V11" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" t="s">
+        <v>13</v>
+      </c>
+      <c r="X11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>775</v>
+      </c>
+      <c r="D12" t="s">
+        <v>788</v>
+      </c>
+      <c r="E12" t="s">
+        <v>802</v>
+      </c>
+      <c r="F12" t="s">
+        <v>777</v>
+      </c>
+      <c r="G12" t="s">
+        <v>830</v>
+      </c>
+      <c r="H12" t="s">
+        <v>847</v>
+      </c>
+      <c r="I12" t="s">
+        <v>845</v>
+      </c>
+      <c r="J12" t="s">
+        <v>879</v>
+      </c>
+      <c r="K12" t="s">
+        <v>896</v>
+      </c>
+      <c r="L12" t="s">
+        <v>909</v>
+      </c>
+      <c r="M12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" t="s">
+        <v>13</v>
+      </c>
+      <c r="U12" t="s">
+        <v>13</v>
+      </c>
+      <c r="V12" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>775</v>
+      </c>
+      <c r="D13" t="s">
+        <v>789</v>
+      </c>
+      <c r="E13" t="s">
+        <v>803</v>
+      </c>
+      <c r="F13" t="s">
+        <v>777</v>
+      </c>
+      <c r="G13" t="s">
+        <v>831</v>
+      </c>
+      <c r="H13" t="s">
+        <v>848</v>
+      </c>
+      <c r="I13" t="s">
+        <v>863</v>
+      </c>
+      <c r="J13" t="s">
+        <v>880</v>
+      </c>
+      <c r="K13" t="s">
+        <v>897</v>
+      </c>
+      <c r="L13" t="s">
+        <v>910</v>
+      </c>
+      <c r="M13" t="s">
+        <v>924</v>
+      </c>
+      <c r="N13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" t="s">
+        <v>13</v>
+      </c>
+      <c r="S13" t="s">
+        <v>13</v>
+      </c>
+      <c r="T13" t="s">
+        <v>13</v>
+      </c>
+      <c r="U13" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" t="s">
+        <v>13</v>
+      </c>
+      <c r="W13" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>775</v>
+      </c>
+      <c r="D14" t="s">
+        <v>790</v>
+      </c>
+      <c r="E14" t="s">
+        <v>804</v>
+      </c>
+      <c r="F14" t="s">
+        <v>777</v>
+      </c>
+      <c r="G14" t="s">
+        <v>832</v>
+      </c>
+      <c r="H14" t="s">
+        <v>849</v>
+      </c>
+      <c r="I14" t="s">
+        <v>866</v>
+      </c>
+      <c r="J14" t="s">
+        <v>881</v>
+      </c>
+      <c r="K14" t="s">
+        <v>898</v>
+      </c>
+      <c r="L14" t="s">
+        <v>848</v>
+      </c>
+      <c r="M14" t="s">
+        <v>843</v>
+      </c>
+      <c r="N14" t="s">
+        <v>935</v>
+      </c>
+      <c r="O14" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R14" t="s">
+        <v>13</v>
+      </c>
+      <c r="S14" t="s">
+        <v>13</v>
+      </c>
+      <c r="T14" t="s">
+        <v>13</v>
+      </c>
+      <c r="U14" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" t="s">
+        <v>13</v>
+      </c>
+      <c r="W14" t="s">
+        <v>13</v>
+      </c>
+      <c r="X14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>776</v>
+      </c>
+      <c r="D15" t="s">
+        <v>779</v>
+      </c>
+      <c r="E15" t="s">
+        <v>805</v>
+      </c>
+      <c r="F15" t="s">
+        <v>817</v>
+      </c>
+      <c r="G15" t="s">
+        <v>833</v>
+      </c>
+      <c r="H15" t="s">
+        <v>850</v>
+      </c>
+      <c r="I15" t="s">
+        <v>867</v>
+      </c>
+      <c r="J15" t="s">
+        <v>882</v>
+      </c>
+      <c r="K15" t="s">
+        <v>899</v>
+      </c>
+      <c r="L15" t="s">
+        <v>911</v>
+      </c>
+      <c r="M15" t="s">
+        <v>925</v>
+      </c>
+      <c r="N15" t="s">
+        <v>936</v>
+      </c>
+      <c r="O15" t="s">
+        <v>945</v>
+      </c>
+      <c r="P15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>13</v>
+      </c>
+      <c r="R15" t="s">
+        <v>13</v>
+      </c>
+      <c r="S15" t="s">
+        <v>13</v>
+      </c>
+      <c r="T15" t="s">
+        <v>13</v>
+      </c>
+      <c r="U15" t="s">
+        <v>13</v>
+      </c>
+      <c r="V15" t="s">
+        <v>13</v>
+      </c>
+      <c r="W15" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>777</v>
+      </c>
+      <c r="D16" t="s">
+        <v>791</v>
+      </c>
+      <c r="E16" t="s">
+        <v>806</v>
+      </c>
+      <c r="F16" t="s">
+        <v>818</v>
+      </c>
+      <c r="G16" t="s">
+        <v>834</v>
+      </c>
+      <c r="H16" t="s">
+        <v>851</v>
+      </c>
+      <c r="I16" t="s">
+        <v>868</v>
+      </c>
+      <c r="J16" t="s">
+        <v>883</v>
+      </c>
+      <c r="K16" t="s">
+        <v>900</v>
+      </c>
+      <c r="L16" t="s">
+        <v>912</v>
+      </c>
+      <c r="M16" t="s">
+        <v>834</v>
+      </c>
+      <c r="N16" t="s">
+        <v>937</v>
+      </c>
+      <c r="O16" t="s">
+        <v>946</v>
+      </c>
+      <c r="P16" t="s">
+        <v>794</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>13</v>
+      </c>
+      <c r="R16" t="s">
+        <v>13</v>
+      </c>
+      <c r="S16" t="s">
+        <v>13</v>
+      </c>
+      <c r="T16" t="s">
+        <v>13</v>
+      </c>
+      <c r="U16" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" t="s">
+        <v>13</v>
+      </c>
+      <c r="W16" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>775</v>
+      </c>
+      <c r="D17" t="s">
+        <v>770</v>
+      </c>
+      <c r="E17" t="s">
+        <v>807</v>
+      </c>
+      <c r="F17" t="s">
+        <v>819</v>
+      </c>
+      <c r="G17" t="s">
+        <v>835</v>
+      </c>
+      <c r="H17" t="s">
+        <v>852</v>
+      </c>
+      <c r="I17" t="s">
+        <v>869</v>
+      </c>
+      <c r="J17" t="s">
+        <v>884</v>
+      </c>
+      <c r="K17" t="s">
+        <v>901</v>
+      </c>
+      <c r="L17" t="s">
+        <v>913</v>
+      </c>
+      <c r="M17" t="s">
+        <v>926</v>
+      </c>
+      <c r="N17" t="s">
+        <v>938</v>
+      </c>
+      <c r="O17" t="s">
+        <v>947</v>
+      </c>
+      <c r="P17" t="s">
+        <v>956</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>965</v>
+      </c>
+      <c r="R17" t="s">
+        <v>13</v>
+      </c>
+      <c r="S17" t="s">
+        <v>13</v>
+      </c>
+      <c r="T17" t="s">
+        <v>13</v>
+      </c>
+      <c r="U17" t="s">
+        <v>13</v>
+      </c>
+      <c r="V17" t="s">
+        <v>13</v>
+      </c>
+      <c r="W17" t="s">
+        <v>13</v>
+      </c>
+      <c r="X17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>778</v>
+      </c>
+      <c r="D18" t="s">
+        <v>792</v>
+      </c>
+      <c r="E18" t="s">
+        <v>808</v>
+      </c>
+      <c r="F18" t="s">
+        <v>820</v>
+      </c>
+      <c r="G18" t="s">
+        <v>836</v>
+      </c>
+      <c r="H18" t="s">
+        <v>853</v>
+      </c>
+      <c r="I18" t="s">
+        <v>870</v>
+      </c>
+      <c r="J18" t="s">
+        <v>885</v>
+      </c>
+      <c r="K18" t="s">
+        <v>902</v>
+      </c>
+      <c r="L18" t="s">
+        <v>798</v>
+      </c>
+      <c r="M18" t="s">
+        <v>927</v>
+      </c>
+      <c r="N18" t="s">
+        <v>845</v>
+      </c>
+      <c r="O18" t="s">
+        <v>948</v>
+      </c>
+      <c r="P18" t="s">
+        <v>957</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>966</v>
+      </c>
+      <c r="R18" t="s">
+        <v>976</v>
+      </c>
+      <c r="S18" t="s">
+        <v>13</v>
+      </c>
+      <c r="T18" t="s">
+        <v>13</v>
+      </c>
+      <c r="U18" t="s">
+        <v>13</v>
+      </c>
+      <c r="V18" t="s">
+        <v>13</v>
+      </c>
+      <c r="W18" t="s">
+        <v>13</v>
+      </c>
+      <c r="X18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>779</v>
+      </c>
+      <c r="D19" t="s">
+        <v>793</v>
+      </c>
+      <c r="E19" t="s">
+        <v>809</v>
+      </c>
+      <c r="F19" t="s">
+        <v>821</v>
+      </c>
+      <c r="G19" t="s">
+        <v>837</v>
+      </c>
+      <c r="H19" t="s">
+        <v>854</v>
+      </c>
+      <c r="I19" t="s">
+        <v>871</v>
+      </c>
+      <c r="J19" t="s">
+        <v>886</v>
+      </c>
+      <c r="K19" t="s">
+        <v>903</v>
+      </c>
+      <c r="L19" t="s">
+        <v>914</v>
+      </c>
+      <c r="M19" t="s">
+        <v>928</v>
+      </c>
+      <c r="N19" t="s">
+        <v>939</v>
+      </c>
+      <c r="O19" t="s">
+        <v>770</v>
+      </c>
+      <c r="P19" t="s">
+        <v>837</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>967</v>
+      </c>
+      <c r="R19" t="s">
+        <v>977</v>
+      </c>
+      <c r="S19" t="s">
+        <v>983</v>
+      </c>
+      <c r="T19" t="s">
+        <v>13</v>
+      </c>
+      <c r="U19" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" t="s">
+        <v>13</v>
+      </c>
+      <c r="W19" t="s">
+        <v>13</v>
+      </c>
+      <c r="X19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>773</v>
+      </c>
+      <c r="D20" t="s">
+        <v>786</v>
+      </c>
+      <c r="E20" t="s">
+        <v>800</v>
+      </c>
+      <c r="F20" t="s">
+        <v>815</v>
+      </c>
+      <c r="G20" t="s">
+        <v>827</v>
+      </c>
+      <c r="H20" t="s">
+        <v>855</v>
+      </c>
+      <c r="I20" t="s">
+        <v>406</v>
+      </c>
+      <c r="J20" t="s">
+        <v>877</v>
+      </c>
+      <c r="K20" t="s">
+        <v>899</v>
+      </c>
+      <c r="L20" t="s">
+        <v>915</v>
+      </c>
+      <c r="M20" t="s">
+        <v>848</v>
+      </c>
+      <c r="N20" t="s">
+        <v>940</v>
+      </c>
+      <c r="O20" t="s">
+        <v>865</v>
+      </c>
+      <c r="P20" t="s">
+        <v>958</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>968</v>
+      </c>
+      <c r="R20" t="s">
+        <v>978</v>
+      </c>
+      <c r="S20" t="s">
+        <v>984</v>
+      </c>
+      <c r="T20" t="s">
+        <v>903</v>
+      </c>
+      <c r="U20" t="s">
+        <v>13</v>
+      </c>
+      <c r="V20" t="s">
+        <v>13</v>
+      </c>
+      <c r="W20" t="s">
+        <v>13</v>
+      </c>
+      <c r="X20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>771</v>
+      </c>
+      <c r="D21" t="s">
+        <v>784</v>
+      </c>
+      <c r="E21" t="s">
+        <v>798</v>
+      </c>
+      <c r="F21" t="s">
+        <v>778</v>
+      </c>
+      <c r="G21" t="s">
+        <v>838</v>
+      </c>
+      <c r="H21" t="s">
+        <v>856</v>
+      </c>
+      <c r="I21" t="s">
+        <v>872</v>
+      </c>
+      <c r="J21" t="s">
+        <v>887</v>
+      </c>
+      <c r="K21" t="s">
+        <v>904</v>
+      </c>
+      <c r="L21" t="s">
+        <v>916</v>
+      </c>
+      <c r="M21" t="s">
+        <v>929</v>
+      </c>
+      <c r="N21" t="s">
+        <v>815</v>
+      </c>
+      <c r="O21" t="s">
+        <v>949</v>
+      </c>
+      <c r="P21" t="s">
+        <v>959</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>969</v>
+      </c>
+      <c r="R21" t="s">
+        <v>814</v>
+      </c>
+      <c r="S21" t="s">
+        <v>861</v>
+      </c>
+      <c r="T21" t="s">
+        <v>854</v>
+      </c>
+      <c r="U21" t="s">
+        <v>785</v>
+      </c>
+      <c r="V21" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" t="s">
+        <v>13</v>
+      </c>
+      <c r="X21" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>772</v>
+      </c>
+      <c r="D22" t="s">
+        <v>785</v>
+      </c>
+      <c r="E22" t="s">
+        <v>799</v>
+      </c>
+      <c r="F22" t="s">
+        <v>814</v>
+      </c>
+      <c r="G22" t="s">
+        <v>839</v>
+      </c>
+      <c r="H22" t="s">
+        <v>857</v>
+      </c>
+      <c r="I22" t="s">
+        <v>873</v>
+      </c>
+      <c r="J22" t="s">
+        <v>888</v>
+      </c>
+      <c r="K22" t="s">
+        <v>888</v>
+      </c>
+      <c r="L22" t="s">
+        <v>917</v>
+      </c>
+      <c r="M22" t="s">
+        <v>930</v>
+      </c>
+      <c r="N22" t="s">
+        <v>803</v>
+      </c>
+      <c r="O22" t="s">
+        <v>950</v>
+      </c>
+      <c r="P22" t="s">
+        <v>960</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>970</v>
+      </c>
+      <c r="R22" t="s">
+        <v>807</v>
+      </c>
+      <c r="S22" t="s">
+        <v>803</v>
+      </c>
+      <c r="T22" t="s">
+        <v>989</v>
+      </c>
+      <c r="U22" t="s">
+        <v>888</v>
+      </c>
+      <c r="V22" t="s">
+        <v>857</v>
+      </c>
+      <c r="W22" t="s">
+        <v>13</v>
+      </c>
+      <c r="X22" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>771</v>
+      </c>
+      <c r="D23" t="s">
+        <v>784</v>
+      </c>
+      <c r="E23" t="s">
+        <v>798</v>
+      </c>
+      <c r="F23" t="s">
+        <v>778</v>
+      </c>
+      <c r="G23" t="s">
+        <v>840</v>
+      </c>
+      <c r="H23" t="s">
+        <v>858</v>
+      </c>
+      <c r="I23" t="s">
+        <v>136</v>
+      </c>
+      <c r="J23" t="s">
+        <v>889</v>
+      </c>
+      <c r="K23" t="s">
+        <v>136</v>
+      </c>
+      <c r="L23" t="s">
+        <v>918</v>
+      </c>
+      <c r="M23" t="s">
+        <v>931</v>
+      </c>
+      <c r="N23" t="s">
+        <v>941</v>
+      </c>
+      <c r="O23" t="s">
+        <v>951</v>
+      </c>
+      <c r="P23" t="s">
+        <v>843</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>971</v>
+      </c>
+      <c r="R23" t="s">
+        <v>863</v>
+      </c>
+      <c r="S23" t="s">
+        <v>845</v>
+      </c>
+      <c r="T23" t="s">
+        <v>990</v>
+      </c>
+      <c r="U23" t="s">
+        <v>996</v>
+      </c>
+      <c r="V23" t="s">
+        <v>999</v>
+      </c>
+      <c r="W23" t="s">
+        <v>887</v>
+      </c>
+      <c r="X23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>780</v>
+      </c>
+      <c r="D24" t="s">
+        <v>794</v>
+      </c>
+      <c r="E24" t="s">
+        <v>810</v>
+      </c>
+      <c r="F24" t="s">
+        <v>822</v>
+      </c>
+      <c r="G24" t="s">
+        <v>773</v>
+      </c>
+      <c r="H24" t="s">
+        <v>859</v>
+      </c>
+      <c r="I24" t="s">
+        <v>874</v>
+      </c>
+      <c r="J24" t="s">
+        <v>890</v>
+      </c>
+      <c r="K24" t="s">
+        <v>905</v>
+      </c>
+      <c r="L24" t="s">
+        <v>919</v>
+      </c>
+      <c r="M24" t="s">
+        <v>932</v>
+      </c>
+      <c r="N24" t="s">
+        <v>942</v>
+      </c>
+      <c r="O24" t="s">
+        <v>952</v>
+      </c>
+      <c r="P24" t="s">
+        <v>961</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>972</v>
+      </c>
+      <c r="R24" t="s">
+        <v>979</v>
+      </c>
+      <c r="S24" t="s">
+        <v>985</v>
+      </c>
+      <c r="T24" t="s">
+        <v>991</v>
+      </c>
+      <c r="U24" t="s">
+        <v>997</v>
+      </c>
+      <c r="V24" t="s">
+        <v>1000</v>
+      </c>
+      <c r="W24" t="s">
+        <v>952</v>
+      </c>
+      <c r="X24" t="s">
+        <v>1005</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>781</v>
+      </c>
+      <c r="D25" t="s">
+        <v>795</v>
+      </c>
+      <c r="E25" t="s">
+        <v>811</v>
+      </c>
+      <c r="F25" t="s">
+        <v>823</v>
+      </c>
+      <c r="G25" t="s">
+        <v>841</v>
+      </c>
+      <c r="H25" t="s">
+        <v>854</v>
+      </c>
+      <c r="I25" t="s">
+        <v>825</v>
+      </c>
+      <c r="J25" t="s">
+        <v>891</v>
+      </c>
+      <c r="K25" t="s">
+        <v>886</v>
+      </c>
+      <c r="L25" t="s">
+        <v>920</v>
+      </c>
+      <c r="M25" t="s">
+        <v>836</v>
+      </c>
+      <c r="N25" t="s">
+        <v>820</v>
+      </c>
+      <c r="O25" t="s">
+        <v>770</v>
+      </c>
+      <c r="P25" t="s">
+        <v>854</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>973</v>
+      </c>
+      <c r="R25" t="s">
+        <v>980</v>
+      </c>
+      <c r="S25" t="s">
+        <v>986</v>
+      </c>
+      <c r="T25" t="s">
+        <v>992</v>
+      </c>
+      <c r="U25" t="s">
+        <v>886</v>
+      </c>
+      <c r="V25" t="s">
+        <v>779</v>
+      </c>
+      <c r="W25" t="s">
+        <v>1002</v>
+      </c>
+      <c r="X25" t="s">
+        <v>1006</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>894</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>772</v>
+      </c>
+      <c r="D26" t="s">
+        <v>785</v>
+      </c>
+      <c r="E26" t="s">
+        <v>799</v>
+      </c>
+      <c r="F26" t="s">
+        <v>814</v>
+      </c>
+      <c r="G26" t="s">
+        <v>812</v>
+      </c>
+      <c r="H26" t="s">
+        <v>860</v>
+      </c>
+      <c r="I26" t="s">
+        <v>875</v>
+      </c>
+      <c r="J26" t="s">
+        <v>892</v>
+      </c>
+      <c r="K26" t="s">
+        <v>906</v>
+      </c>
+      <c r="L26" t="s">
+        <v>921</v>
+      </c>
+      <c r="M26" t="s">
+        <v>933</v>
+      </c>
+      <c r="N26" t="s">
+        <v>943</v>
+      </c>
+      <c r="O26" t="s">
+        <v>953</v>
+      </c>
+      <c r="P26" t="s">
+        <v>962</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>974</v>
+      </c>
+      <c r="R26" t="s">
+        <v>981</v>
+      </c>
+      <c r="S26" t="s">
+        <v>893</v>
+      </c>
+      <c r="T26" t="s">
+        <v>993</v>
+      </c>
+      <c r="U26" t="s">
+        <v>801</v>
+      </c>
+      <c r="V26" t="s">
+        <v>1001</v>
+      </c>
+      <c r="W26" t="s">
+        <v>1003</v>
+      </c>
+      <c r="X26" t="s">
+        <v>1007</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>1009</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>1012</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>778</v>
+      </c>
+      <c r="D27" t="s">
+        <v>792</v>
+      </c>
+      <c r="E27" t="s">
+        <v>808</v>
+      </c>
+      <c r="F27" t="s">
+        <v>820</v>
+      </c>
+      <c r="G27" t="s">
+        <v>836</v>
+      </c>
+      <c r="H27" t="s">
+        <v>861</v>
+      </c>
+      <c r="I27" t="s">
+        <v>876</v>
+      </c>
+      <c r="J27" t="s">
+        <v>893</v>
+      </c>
+      <c r="K27" t="s">
+        <v>907</v>
+      </c>
+      <c r="L27" t="s">
+        <v>922</v>
+      </c>
+      <c r="M27" t="s">
+        <v>934</v>
+      </c>
+      <c r="N27" t="s">
+        <v>944</v>
+      </c>
+      <c r="O27" t="s">
+        <v>954</v>
+      </c>
+      <c r="P27" t="s">
+        <v>963</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>967</v>
+      </c>
+      <c r="R27" t="s">
+        <v>982</v>
+      </c>
+      <c r="S27" t="s">
+        <v>987</v>
+      </c>
+      <c r="T27" t="s">
+        <v>994</v>
+      </c>
+      <c r="U27" t="s">
+        <v>907</v>
+      </c>
+      <c r="V27" t="s">
+        <v>861</v>
+      </c>
+      <c r="W27" t="s">
+        <v>858</v>
+      </c>
+      <c r="X27" t="s">
+        <v>876</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>1010</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>803</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>782</v>
+      </c>
+      <c r="D28" t="s">
+        <v>796</v>
+      </c>
+      <c r="E28" t="s">
+        <v>812</v>
+      </c>
+      <c r="F28" t="s">
+        <v>824</v>
+      </c>
+      <c r="G28" t="s">
+        <v>842</v>
+      </c>
+      <c r="H28" t="s">
+        <v>862</v>
+      </c>
+      <c r="I28" t="s">
+        <v>783</v>
+      </c>
+      <c r="J28" t="s">
+        <v>894</v>
+      </c>
+      <c r="K28" t="s">
+        <v>908</v>
+      </c>
+      <c r="L28" t="s">
+        <v>923</v>
+      </c>
+      <c r="M28" t="s">
+        <v>834</v>
+      </c>
+      <c r="N28" t="s">
+        <v>781</v>
+      </c>
+      <c r="O28" t="s">
+        <v>955</v>
+      </c>
+      <c r="P28" t="s">
+        <v>964</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>975</v>
+      </c>
+      <c r="R28" t="s">
+        <v>837</v>
+      </c>
+      <c r="S28" t="s">
+        <v>988</v>
+      </c>
+      <c r="T28" t="s">
+        <v>995</v>
+      </c>
+      <c r="U28" t="s">
+        <v>998</v>
+      </c>
+      <c r="V28" t="s">
+        <v>770</v>
+      </c>
+      <c r="W28" t="s">
+        <v>1004</v>
+      </c>
+      <c r="X28" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>1011</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>1014</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>1015</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new stem age scripts, data, results, and update old scripts to remove phi fd
</commit_message>
<xml_diff>
--- a/02_pam/output/stat_results/pairwise_allmetsxtissues.xlsx
+++ b/02_pam/output/stat_results/pairwise_allmetsxtissues.xlsx
@@ -9,13 +9,12 @@
     <sheet name="Fv.Fm" r:id="rId3" sheetId="1"/>
     <sheet name="φPSII" r:id="rId4" sheetId="2"/>
     <sheet name="ΦNPQ" r:id="rId5" sheetId="3"/>
-    <sheet name="Φf.D" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3124" uniqueCount="1017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="770">
   <si>
     <t/>
   </si>
@@ -2325,747 +2324,6 @@
   </si>
   <si>
     <t>0.0269582458724946</t>
-  </si>
-  <si>
-    <t>1.46914413092828e-06</t>
-  </si>
-  <si>
-    <t>1.97325911664838e-06</t>
-  </si>
-  <si>
-    <t>1.37582108242688e-05</t>
-  </si>
-  <si>
-    <t>1.89780302773899e-05</t>
-  </si>
-  <si>
-    <t>0.000102924586269731</t>
-  </si>
-  <si>
-    <t>4.84504487856965e-10</t>
-  </si>
-  <si>
-    <t>4.27413716681936e-09</t>
-  </si>
-  <si>
-    <t>6.85417095264142e-09</t>
-  </si>
-  <si>
-    <t>6.66841770080943e-06</t>
-  </si>
-  <si>
-    <t>2.98707480394053e-06</t>
-  </si>
-  <si>
-    <t>3.91284878298995e-06</t>
-  </si>
-  <si>
-    <t>2.39181431914157e-06</t>
-  </si>
-  <si>
-    <t>1.62974558250254e-06</t>
-  </si>
-  <si>
-    <t>6.47760868396346e-05</t>
-  </si>
-  <si>
-    <t>8.8306053652654e-05</t>
-  </si>
-  <si>
-    <t>0.000550670992849549</t>
-  </si>
-  <si>
-    <t>0.00077123100333586</t>
-  </si>
-  <si>
-    <t>0.00223525342731377</t>
-  </si>
-  <si>
-    <t>1.59711047350042e-06</t>
-  </si>
-  <si>
-    <t>1.52781452914049e-06</t>
-  </si>
-  <si>
-    <t>1.59002101370314e-06</t>
-  </si>
-  <si>
-    <t>4.11268967627329e-06</t>
-  </si>
-  <si>
-    <t>0.000298172236159297</t>
-  </si>
-  <si>
-    <t>0.000137871385547842</t>
-  </si>
-  <si>
-    <t>0.000177368594616916</t>
-  </si>
-  <si>
-    <t>0.000108960165287834</t>
-  </si>
-  <si>
-    <t>7.60220907448281e-05</t>
-  </si>
-  <si>
-    <t>0.00517725139988128</t>
-  </si>
-  <si>
-    <t>0.00600173139632833</t>
-  </si>
-  <si>
-    <t>0.0172760588303928</t>
-  </si>
-  <si>
-    <t>0.0225198353259596</t>
-  </si>
-  <si>
-    <t>0.0432006010518407</t>
-  </si>
-  <si>
-    <t>0.00133843987321872</t>
-  </si>
-  <si>
-    <t>0.00132102267310655</t>
-  </si>
-  <si>
-    <t>0.00133443791013325</t>
-  </si>
-  <si>
-    <t>0.0016770568502043</t>
-  </si>
-  <si>
-    <t>0.00183777596266874</t>
-  </si>
-  <si>
-    <t>0.00131826197442768</t>
-  </si>
-  <si>
-    <t>0.0113964152253623</t>
-  </si>
-  <si>
-    <t>0.00737904307983945</t>
-  </si>
-  <si>
-    <t>0.00830318766008975</t>
-  </si>
-  <si>
-    <t>0.00665913303636113</t>
-  </si>
-  <si>
-    <t>0.00557432501490154</t>
-  </si>
-  <si>
-    <t>4.64475228235315e-06</t>
-  </si>
-  <si>
-    <t>5.00452061270906e-05</t>
-  </si>
-  <si>
-    <t>7.09662241449245e-05</t>
-  </si>
-  <si>
-    <t>0.000319870256601466</t>
-  </si>
-  <si>
-    <t>4.10307004148575e-08</t>
-  </si>
-  <si>
-    <t>8.181227864492e-08</t>
-  </si>
-  <si>
-    <t>6.8431245413214e-09</t>
-  </si>
-  <si>
-    <t>2.58926676774888e-05</t>
-  </si>
-  <si>
-    <t>1.15693532316023e-05</t>
-  </si>
-  <si>
-    <t>1.49691494917964e-05</t>
-  </si>
-  <si>
-    <t>8.57887930232797e-06</t>
-  </si>
-  <si>
-    <t>5.55167945084225e-06</t>
-  </si>
-  <si>
-    <t>0.000965878342183555</t>
-  </si>
-  <si>
-    <t>0.0147743541861189</t>
-  </si>
-  <si>
-    <t>0.000593395252837977</t>
-  </si>
-  <si>
-    <t>0.00107240105934574</t>
-  </si>
-  <si>
-    <t>0.52747462724168</t>
-  </si>
-  <si>
-    <t>0.00427981982827575</t>
-  </si>
-  <si>
-    <t>3.45421735272256e-06</t>
-  </si>
-  <si>
-    <t>0.00262153063538664</t>
-  </si>
-  <si>
-    <t>7.33593486161674e-05</t>
-  </si>
-  <si>
-    <t>8.42421556876668e-07</t>
-  </si>
-  <si>
-    <t>2.51535316335364e-06</t>
-  </si>
-  <si>
-    <t>1.8516598278697e-05</t>
-  </si>
-  <si>
-    <t>2.35018362768078e-06</t>
-  </si>
-  <si>
-    <t>0.228276520946051</t>
-  </si>
-  <si>
-    <t>0.000106853887065662</t>
-  </si>
-  <si>
-    <t>2.234446410143e-05</t>
-  </si>
-  <si>
-    <t>1.47007370949579e-06</t>
-  </si>
-  <si>
-    <t>5.2332238542903e-07</t>
-  </si>
-  <si>
-    <t>0.41235784569169</t>
-  </si>
-  <si>
-    <t>0.255118170322243</t>
-  </si>
-  <si>
-    <t>0.388475000884946</t>
-  </si>
-  <si>
-    <t>0.12278132410577</t>
-  </si>
-  <si>
-    <t>0.640435177013749</t>
-  </si>
-  <si>
-    <t>0.222615143447838</t>
-  </si>
-  <si>
-    <t>0.25369823416405</t>
-  </si>
-  <si>
-    <t>0.537341519813543</t>
-  </si>
-  <si>
-    <t>0.0045654971008991</t>
-  </si>
-  <si>
-    <t>0.110588172516772</t>
-  </si>
-  <si>
-    <t>0.074108019872502</t>
-  </si>
-  <si>
-    <t>5.02593381850348e-06</t>
-  </si>
-  <si>
-    <t>0.219983213873785</t>
-  </si>
-  <si>
-    <t>0.0040934555640438</t>
-  </si>
-  <si>
-    <t>0.000197141280012617</t>
-  </si>
-  <si>
-    <t>0.108231536802965</t>
-  </si>
-  <si>
-    <t>0.0221623928817677</t>
-  </si>
-  <si>
-    <t>0.63199813569665</t>
-  </si>
-  <si>
-    <t>3.76758890690779e-05</t>
-  </si>
-  <si>
-    <t>2.99128041758275e-06</t>
-  </si>
-  <si>
-    <t>0.974917263444279</t>
-  </si>
-  <si>
-    <t>0.882215838142486</t>
-  </si>
-  <si>
-    <t>0.034830859675753</t>
-  </si>
-  <si>
-    <t>0.109778968979575</t>
-  </si>
-  <si>
-    <t>0.653001970257221</t>
-  </si>
-  <si>
-    <t>0.109525839900054</t>
-  </si>
-  <si>
-    <t>0.864218292792991</t>
-  </si>
-  <si>
-    <t>0.890596921556674</t>
-  </si>
-  <si>
-    <t>5.35928657177157e-05</t>
-  </si>
-  <si>
-    <t>0.0547114833854163</t>
-  </si>
-  <si>
-    <t>0.00548516620270399</t>
-  </si>
-  <si>
-    <t>0.500991631476399</t>
-  </si>
-  <si>
-    <t>0.334101627628805</t>
-  </si>
-  <si>
-    <t>0.000186896142626135</t>
-  </si>
-  <si>
-    <t>0.950011526934604</t>
-  </si>
-  <si>
-    <t>0.0409350408715385</t>
-  </si>
-  <si>
-    <t>0.2260744260024</t>
-  </si>
-  <si>
-    <t>0.77746080472901</t>
-  </si>
-  <si>
-    <t>0.0417671141674737</t>
-  </si>
-  <si>
-    <t>0.578977984401115</t>
-  </si>
-  <si>
-    <t>0.311955015353317</t>
-  </si>
-  <si>
-    <t>0.911188557904474</t>
-  </si>
-  <si>
-    <t>0.544503727783471</t>
-  </si>
-  <si>
-    <t>0.000719394457534875</t>
-  </si>
-  <si>
-    <t>0.000669242766358621</t>
-  </si>
-  <si>
-    <t>0.00694654183026276</t>
-  </si>
-  <si>
-    <t>0.866582441531232</t>
-  </si>
-  <si>
-    <t>0.417214364582786</t>
-  </si>
-  <si>
-    <t>0.00362156696998326</t>
-  </si>
-  <si>
-    <t>0.0881992023724307</t>
-  </si>
-  <si>
-    <t>0.00243143100285957</t>
-  </si>
-  <si>
-    <t>0.000496472052199606</t>
-  </si>
-  <si>
-    <t>0.0516966014153839</t>
-  </si>
-  <si>
-    <t>0.351062497502936</t>
-  </si>
-  <si>
-    <t>0.981920658565482</t>
-  </si>
-  <si>
-    <t>0.0848304556751086</t>
-  </si>
-  <si>
-    <t>0.7375055285272</t>
-  </si>
-  <si>
-    <t>0.230206278613672</t>
-  </si>
-  <si>
-    <t>0.85878008001157</t>
-  </si>
-  <si>
-    <t>0.407459207459207</t>
-  </si>
-  <si>
-    <t>0.000969122901638239</t>
-  </si>
-  <si>
-    <t>0.00177971741182661</t>
-  </si>
-  <si>
-    <t>0.252584295137487</t>
-  </si>
-  <si>
-    <t>0.0722664432341852</t>
-  </si>
-  <si>
-    <t>0.00279234654234654</t>
-  </si>
-  <si>
-    <t>0.00134100622110277</t>
-  </si>
-  <si>
-    <t>0.0996880698288051</t>
-  </si>
-  <si>
-    <t>0.00174043475952857</t>
-  </si>
-  <si>
-    <t>0.0117911941505956</t>
-  </si>
-  <si>
-    <t>8.03429624641099e-05</t>
-  </si>
-  <si>
-    <t>0.000836085352458897</t>
-  </si>
-  <si>
-    <t>8.36615342040886e-05</t>
-  </si>
-  <si>
-    <t>0.0262486400669766</t>
-  </si>
-  <si>
-    <t>0.830142079839557</t>
-  </si>
-  <si>
-    <t>0.00122051474373625</t>
-  </si>
-  <si>
-    <t>0.00818806614326521</t>
-  </si>
-  <si>
-    <t>0.00212395364263973</t>
-  </si>
-  <si>
-    <t>5.83597508868402e-05</t>
-  </si>
-  <si>
-    <t>0.435133539653415</t>
-  </si>
-  <si>
-    <t>0.000363574791533674</t>
-  </si>
-  <si>
-    <t>4.17275545299923e-05</t>
-  </si>
-  <si>
-    <t>0.000459598735533525</t>
-  </si>
-  <si>
-    <t>0.138777614747971</t>
-  </si>
-  <si>
-    <t>8.6069514601272e-05</t>
-  </si>
-  <si>
-    <t>0.0942214438995076</t>
-  </si>
-  <si>
-    <t>3.21798807942617e-06</t>
-  </si>
-  <si>
-    <t>0.141236795572487</t>
-  </si>
-  <si>
-    <t>0.00124685894135588</t>
-  </si>
-  <si>
-    <t>0.0828422289728547</t>
-  </si>
-  <si>
-    <t>0.024109968720655</t>
-  </si>
-  <si>
-    <t>0.95643846763465</t>
-  </si>
-  <si>
-    <t>3.59798854605734e-05</t>
-  </si>
-  <si>
-    <t>4.88419660941623e-07</t>
-  </si>
-  <si>
-    <t>0.249374085071198</t>
-  </si>
-  <si>
-    <t>0.000724345474603722</t>
-  </si>
-  <si>
-    <t>0.450068987877592</t>
-  </si>
-  <si>
-    <t>7.17444463607316e-06</t>
-  </si>
-  <si>
-    <t>0.71934741622644</t>
-  </si>
-  <si>
-    <t>0.745878483582455</t>
-  </si>
-  <si>
-    <t>0.156722031545248</t>
-  </si>
-  <si>
-    <t>0.147698585718734</t>
-  </si>
-  <si>
-    <t>5.88473289567701e-05</t>
-  </si>
-  <si>
-    <t>0.00316811062959207</t>
-  </si>
-  <si>
-    <t>7.45115564620668e-10</t>
-  </si>
-  <si>
-    <t>1.0376690000045e-08</t>
-  </si>
-  <si>
-    <t>0.00476209352547718</t>
-  </si>
-  <si>
-    <t>0.0656128394634793</t>
-  </si>
-  <si>
-    <t>0.000230231294633637</t>
-  </si>
-  <si>
-    <t>0.00448562766171116</t>
-  </si>
-  <si>
-    <t>0.00104441013531923</t>
-  </si>
-  <si>
-    <t>0.666824197433516</t>
-  </si>
-  <si>
-    <t>1.8033773890489e-05</t>
-  </si>
-  <si>
-    <t>8.36382575950447e-08</t>
-  </si>
-  <si>
-    <t>0.0777192882398123</t>
-  </si>
-  <si>
-    <t>0.199594619511259</t>
-  </si>
-  <si>
-    <t>0.558104168502009</t>
-  </si>
-  <si>
-    <t>0.0032490636913743</t>
-  </si>
-  <si>
-    <t>0.000406129779755323</t>
-  </si>
-  <si>
-    <t>0.0606599056262665</t>
-  </si>
-  <si>
-    <t>0.306165580092081</t>
-  </si>
-  <si>
-    <t>2.8813221974895e-05</t>
-  </si>
-  <si>
-    <t>1.08163834329771e-06</t>
-  </si>
-  <si>
-    <t>0.00375000514523381</t>
-  </si>
-  <si>
-    <t>0.384601566106412</t>
-  </si>
-  <si>
-    <t>0.00219649485233478</t>
-  </si>
-  <si>
-    <t>0.376112227389182</t>
-  </si>
-  <si>
-    <t>2.44964602326803e-06</t>
-  </si>
-  <si>
-    <t>0.0775251638891432</t>
-  </si>
-  <si>
-    <t>0.123343827541559</t>
-  </si>
-  <si>
-    <t>0.543179232716163</t>
-  </si>
-  <si>
-    <t>0.0328143114148778</t>
-  </si>
-  <si>
-    <t>0.0108845806136957</t>
-  </si>
-  <si>
-    <t>0.00135531591429068</t>
-  </si>
-  <si>
-    <t>0.670219962050164</t>
-  </si>
-  <si>
-    <t>7.87148294906324e-06</t>
-  </si>
-  <si>
-    <t>0.936014987115839</t>
-  </si>
-  <si>
-    <t>0.280338586097211</t>
-  </si>
-  <si>
-    <t>4.08078070189144e-05</t>
-  </si>
-  <si>
-    <t>0.0673417303503099</t>
-  </si>
-  <si>
-    <t>6.43818589541128e-05</t>
-  </si>
-  <si>
-    <t>8.22446642880079e-05</t>
-  </si>
-  <si>
-    <t>0.335999616821535</t>
-  </si>
-  <si>
-    <t>0.627137568314039</t>
-  </si>
-  <si>
-    <t>5.53282287028417e-05</t>
-  </si>
-  <si>
-    <t>0.000385705421676645</t>
-  </si>
-  <si>
-    <t>0.00019918162333023</t>
-  </si>
-  <si>
-    <t>0.22442120419398</t>
-  </si>
-  <si>
-    <t>2.38886977793067e-05</t>
-  </si>
-  <si>
-    <t>4.20698513178289e-05</t>
-  </si>
-  <si>
-    <t>0.106360192433123</t>
-  </si>
-  <si>
-    <t>0.000398236217563949</t>
-  </si>
-  <si>
-    <t>0.285548602772797</t>
-  </si>
-  <si>
-    <t>0.771457489878543</t>
-  </si>
-  <si>
-    <t>0.555982008187891</t>
-  </si>
-  <si>
-    <t>0.30476467976468</t>
-  </si>
-  <si>
-    <t>0.00223320794078809</t>
-  </si>
-  <si>
-    <t>1.75070028011205e-05</t>
-  </si>
-  <si>
-    <t>2.83817439162549e-05</t>
-  </si>
-  <si>
-    <t>0.00750045349209293</t>
-  </si>
-  <si>
-    <t>0.791568568147089</t>
-  </si>
-  <si>
-    <t>0.00379062561803679</t>
-  </si>
-  <si>
-    <t>0.223232714138287</t>
-  </si>
-  <si>
-    <t>0.280330717026171</t>
-  </si>
-  <si>
-    <t>0.000360282414925248</t>
-  </si>
-  <si>
-    <t>0.0411794314730957</t>
-  </si>
-  <si>
-    <t>1.47427392009435e-05</t>
-  </si>
-  <si>
-    <t>0.00750969214271967</t>
-  </si>
-  <si>
-    <t>0.000238917351216816</t>
-  </si>
-  <si>
-    <t>0.000130840425853603</t>
-  </si>
-  <si>
-    <t>0.000279464012325578</t>
-  </si>
-  <si>
-    <t>0.0367477488612418</t>
-  </si>
-  <si>
-    <t>0.18500171998624</t>
-  </si>
-  <si>
-    <t>0.000144730549472677</t>
-  </si>
-  <si>
-    <t>0.142107757928539</t>
   </si>
 </sst>
 </file>
@@ -10369,2425 +9627,4 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V1" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" t="s">
-        <v>10</v>
-      </c>
-      <c r="W2" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U3" t="s">
-        <v>13</v>
-      </c>
-      <c r="V3" t="s">
-        <v>13</v>
-      </c>
-      <c r="W3" t="s">
-        <v>13</v>
-      </c>
-      <c r="X3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" t="s">
-        <v>13</v>
-      </c>
-      <c r="S4" t="s">
-        <v>13</v>
-      </c>
-      <c r="T4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" t="s">
-        <v>13</v>
-      </c>
-      <c r="P5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>13</v>
-      </c>
-      <c r="R5" t="s">
-        <v>13</v>
-      </c>
-      <c r="S5" t="s">
-        <v>13</v>
-      </c>
-      <c r="T5" t="s">
-        <v>13</v>
-      </c>
-      <c r="U5" t="s">
-        <v>13</v>
-      </c>
-      <c r="V5" t="s">
-        <v>13</v>
-      </c>
-      <c r="W5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>770</v>
-      </c>
-      <c r="D6" t="s">
-        <v>783</v>
-      </c>
-      <c r="E6" t="s">
-        <v>797</v>
-      </c>
-      <c r="F6" t="s">
-        <v>813</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" t="s">
-        <v>13</v>
-      </c>
-      <c r="S6" t="s">
-        <v>13</v>
-      </c>
-      <c r="T6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W6" t="s">
-        <v>13</v>
-      </c>
-      <c r="X6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>771</v>
-      </c>
-      <c r="D7" t="s">
-        <v>784</v>
-      </c>
-      <c r="E7" t="s">
-        <v>798</v>
-      </c>
-      <c r="F7" t="s">
-        <v>778</v>
-      </c>
-      <c r="G7" t="s">
-        <v>825</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" t="s">
-        <v>13</v>
-      </c>
-      <c r="O7" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>13</v>
-      </c>
-      <c r="R7" t="s">
-        <v>13</v>
-      </c>
-      <c r="S7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T7" t="s">
-        <v>13</v>
-      </c>
-      <c r="U7" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>771</v>
-      </c>
-      <c r="D8" t="s">
-        <v>784</v>
-      </c>
-      <c r="E8" t="s">
-        <v>798</v>
-      </c>
-      <c r="F8" t="s">
-        <v>778</v>
-      </c>
-      <c r="G8" t="s">
-        <v>826</v>
-      </c>
-      <c r="H8" t="s">
-        <v>843</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>13</v>
-      </c>
-      <c r="R8" t="s">
-        <v>13</v>
-      </c>
-      <c r="S8" t="s">
-        <v>13</v>
-      </c>
-      <c r="T8" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" t="s">
-        <v>13</v>
-      </c>
-      <c r="V8" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>772</v>
-      </c>
-      <c r="D9" t="s">
-        <v>785</v>
-      </c>
-      <c r="E9" t="s">
-        <v>799</v>
-      </c>
-      <c r="F9" t="s">
-        <v>814</v>
-      </c>
-      <c r="G9" t="s">
-        <v>827</v>
-      </c>
-      <c r="H9" t="s">
-        <v>844</v>
-      </c>
-      <c r="I9" t="s">
-        <v>863</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N9" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" t="s">
-        <v>13</v>
-      </c>
-      <c r="P9" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>13</v>
-      </c>
-      <c r="R9" t="s">
-        <v>13</v>
-      </c>
-      <c r="S9" t="s">
-        <v>13</v>
-      </c>
-      <c r="T9" t="s">
-        <v>13</v>
-      </c>
-      <c r="U9" t="s">
-        <v>13</v>
-      </c>
-      <c r="V9" t="s">
-        <v>13</v>
-      </c>
-      <c r="W9" t="s">
-        <v>13</v>
-      </c>
-      <c r="X9" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>773</v>
-      </c>
-      <c r="D10" t="s">
-        <v>786</v>
-      </c>
-      <c r="E10" t="s">
-        <v>800</v>
-      </c>
-      <c r="F10" t="s">
-        <v>815</v>
-      </c>
-      <c r="G10" t="s">
-        <v>828</v>
-      </c>
-      <c r="H10" t="s">
-        <v>845</v>
-      </c>
-      <c r="I10" t="s">
-        <v>864</v>
-      </c>
-      <c r="J10" t="s">
-        <v>877</v>
-      </c>
-      <c r="K10" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" t="s">
-        <v>13</v>
-      </c>
-      <c r="O10" t="s">
-        <v>13</v>
-      </c>
-      <c r="P10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R10" t="s">
-        <v>13</v>
-      </c>
-      <c r="S10" t="s">
-        <v>13</v>
-      </c>
-      <c r="T10" t="s">
-        <v>13</v>
-      </c>
-      <c r="U10" t="s">
-        <v>13</v>
-      </c>
-      <c r="V10" t="s">
-        <v>13</v>
-      </c>
-      <c r="W10" t="s">
-        <v>13</v>
-      </c>
-      <c r="X10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>774</v>
-      </c>
-      <c r="D11" t="s">
-        <v>787</v>
-      </c>
-      <c r="E11" t="s">
-        <v>801</v>
-      </c>
-      <c r="F11" t="s">
-        <v>816</v>
-      </c>
-      <c r="G11" t="s">
-        <v>829</v>
-      </c>
-      <c r="H11" t="s">
-        <v>846</v>
-      </c>
-      <c r="I11" t="s">
-        <v>865</v>
-      </c>
-      <c r="J11" t="s">
-        <v>878</v>
-      </c>
-      <c r="K11" t="s">
-        <v>895</v>
-      </c>
-      <c r="L11" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" t="s">
-        <v>13</v>
-      </c>
-      <c r="N11" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" t="s">
-        <v>13</v>
-      </c>
-      <c r="P11" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>13</v>
-      </c>
-      <c r="R11" t="s">
-        <v>13</v>
-      </c>
-      <c r="S11" t="s">
-        <v>13</v>
-      </c>
-      <c r="T11" t="s">
-        <v>13</v>
-      </c>
-      <c r="U11" t="s">
-        <v>13</v>
-      </c>
-      <c r="V11" t="s">
-        <v>13</v>
-      </c>
-      <c r="W11" t="s">
-        <v>13</v>
-      </c>
-      <c r="X11" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>775</v>
-      </c>
-      <c r="D12" t="s">
-        <v>788</v>
-      </c>
-      <c r="E12" t="s">
-        <v>802</v>
-      </c>
-      <c r="F12" t="s">
-        <v>777</v>
-      </c>
-      <c r="G12" t="s">
-        <v>830</v>
-      </c>
-      <c r="H12" t="s">
-        <v>847</v>
-      </c>
-      <c r="I12" t="s">
-        <v>845</v>
-      </c>
-      <c r="J12" t="s">
-        <v>879</v>
-      </c>
-      <c r="K12" t="s">
-        <v>896</v>
-      </c>
-      <c r="L12" t="s">
-        <v>909</v>
-      </c>
-      <c r="M12" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" t="s">
-        <v>13</v>
-      </c>
-      <c r="P12" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>13</v>
-      </c>
-      <c r="R12" t="s">
-        <v>13</v>
-      </c>
-      <c r="S12" t="s">
-        <v>13</v>
-      </c>
-      <c r="T12" t="s">
-        <v>13</v>
-      </c>
-      <c r="U12" t="s">
-        <v>13</v>
-      </c>
-      <c r="V12" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>775</v>
-      </c>
-      <c r="D13" t="s">
-        <v>789</v>
-      </c>
-      <c r="E13" t="s">
-        <v>803</v>
-      </c>
-      <c r="F13" t="s">
-        <v>777</v>
-      </c>
-      <c r="G13" t="s">
-        <v>831</v>
-      </c>
-      <c r="H13" t="s">
-        <v>848</v>
-      </c>
-      <c r="I13" t="s">
-        <v>863</v>
-      </c>
-      <c r="J13" t="s">
-        <v>880</v>
-      </c>
-      <c r="K13" t="s">
-        <v>897</v>
-      </c>
-      <c r="L13" t="s">
-        <v>910</v>
-      </c>
-      <c r="M13" t="s">
-        <v>924</v>
-      </c>
-      <c r="N13" t="s">
-        <v>13</v>
-      </c>
-      <c r="O13" t="s">
-        <v>13</v>
-      </c>
-      <c r="P13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>13</v>
-      </c>
-      <c r="R13" t="s">
-        <v>13</v>
-      </c>
-      <c r="S13" t="s">
-        <v>13</v>
-      </c>
-      <c r="T13" t="s">
-        <v>13</v>
-      </c>
-      <c r="U13" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" t="s">
-        <v>13</v>
-      </c>
-      <c r="W13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>775</v>
-      </c>
-      <c r="D14" t="s">
-        <v>790</v>
-      </c>
-      <c r="E14" t="s">
-        <v>804</v>
-      </c>
-      <c r="F14" t="s">
-        <v>777</v>
-      </c>
-      <c r="G14" t="s">
-        <v>832</v>
-      </c>
-      <c r="H14" t="s">
-        <v>849</v>
-      </c>
-      <c r="I14" t="s">
-        <v>866</v>
-      </c>
-      <c r="J14" t="s">
-        <v>881</v>
-      </c>
-      <c r="K14" t="s">
-        <v>898</v>
-      </c>
-      <c r="L14" t="s">
-        <v>848</v>
-      </c>
-      <c r="M14" t="s">
-        <v>843</v>
-      </c>
-      <c r="N14" t="s">
-        <v>935</v>
-      </c>
-      <c r="O14" t="s">
-        <v>13</v>
-      </c>
-      <c r="P14" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>13</v>
-      </c>
-      <c r="R14" t="s">
-        <v>13</v>
-      </c>
-      <c r="S14" t="s">
-        <v>13</v>
-      </c>
-      <c r="T14" t="s">
-        <v>13</v>
-      </c>
-      <c r="U14" t="s">
-        <v>13</v>
-      </c>
-      <c r="V14" t="s">
-        <v>13</v>
-      </c>
-      <c r="W14" t="s">
-        <v>13</v>
-      </c>
-      <c r="X14" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>776</v>
-      </c>
-      <c r="D15" t="s">
-        <v>779</v>
-      </c>
-      <c r="E15" t="s">
-        <v>805</v>
-      </c>
-      <c r="F15" t="s">
-        <v>817</v>
-      </c>
-      <c r="G15" t="s">
-        <v>833</v>
-      </c>
-      <c r="H15" t="s">
-        <v>850</v>
-      </c>
-      <c r="I15" t="s">
-        <v>867</v>
-      </c>
-      <c r="J15" t="s">
-        <v>882</v>
-      </c>
-      <c r="K15" t="s">
-        <v>899</v>
-      </c>
-      <c r="L15" t="s">
-        <v>911</v>
-      </c>
-      <c r="M15" t="s">
-        <v>925</v>
-      </c>
-      <c r="N15" t="s">
-        <v>936</v>
-      </c>
-      <c r="O15" t="s">
-        <v>945</v>
-      </c>
-      <c r="P15" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>13</v>
-      </c>
-      <c r="R15" t="s">
-        <v>13</v>
-      </c>
-      <c r="S15" t="s">
-        <v>13</v>
-      </c>
-      <c r="T15" t="s">
-        <v>13</v>
-      </c>
-      <c r="U15" t="s">
-        <v>13</v>
-      </c>
-      <c r="V15" t="s">
-        <v>13</v>
-      </c>
-      <c r="W15" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>777</v>
-      </c>
-      <c r="D16" t="s">
-        <v>791</v>
-      </c>
-      <c r="E16" t="s">
-        <v>806</v>
-      </c>
-      <c r="F16" t="s">
-        <v>818</v>
-      </c>
-      <c r="G16" t="s">
-        <v>834</v>
-      </c>
-      <c r="H16" t="s">
-        <v>851</v>
-      </c>
-      <c r="I16" t="s">
-        <v>868</v>
-      </c>
-      <c r="J16" t="s">
-        <v>883</v>
-      </c>
-      <c r="K16" t="s">
-        <v>900</v>
-      </c>
-      <c r="L16" t="s">
-        <v>912</v>
-      </c>
-      <c r="M16" t="s">
-        <v>834</v>
-      </c>
-      <c r="N16" t="s">
-        <v>937</v>
-      </c>
-      <c r="O16" t="s">
-        <v>946</v>
-      </c>
-      <c r="P16" t="s">
-        <v>794</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>13</v>
-      </c>
-      <c r="R16" t="s">
-        <v>13</v>
-      </c>
-      <c r="S16" t="s">
-        <v>13</v>
-      </c>
-      <c r="T16" t="s">
-        <v>13</v>
-      </c>
-      <c r="U16" t="s">
-        <v>13</v>
-      </c>
-      <c r="V16" t="s">
-        <v>13</v>
-      </c>
-      <c r="W16" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>775</v>
-      </c>
-      <c r="D17" t="s">
-        <v>770</v>
-      </c>
-      <c r="E17" t="s">
-        <v>807</v>
-      </c>
-      <c r="F17" t="s">
-        <v>819</v>
-      </c>
-      <c r="G17" t="s">
-        <v>835</v>
-      </c>
-      <c r="H17" t="s">
-        <v>852</v>
-      </c>
-      <c r="I17" t="s">
-        <v>869</v>
-      </c>
-      <c r="J17" t="s">
-        <v>884</v>
-      </c>
-      <c r="K17" t="s">
-        <v>901</v>
-      </c>
-      <c r="L17" t="s">
-        <v>913</v>
-      </c>
-      <c r="M17" t="s">
-        <v>926</v>
-      </c>
-      <c r="N17" t="s">
-        <v>938</v>
-      </c>
-      <c r="O17" t="s">
-        <v>947</v>
-      </c>
-      <c r="P17" t="s">
-        <v>956</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>965</v>
-      </c>
-      <c r="R17" t="s">
-        <v>13</v>
-      </c>
-      <c r="S17" t="s">
-        <v>13</v>
-      </c>
-      <c r="T17" t="s">
-        <v>13</v>
-      </c>
-      <c r="U17" t="s">
-        <v>13</v>
-      </c>
-      <c r="V17" t="s">
-        <v>13</v>
-      </c>
-      <c r="W17" t="s">
-        <v>13</v>
-      </c>
-      <c r="X17" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>778</v>
-      </c>
-      <c r="D18" t="s">
-        <v>792</v>
-      </c>
-      <c r="E18" t="s">
-        <v>808</v>
-      </c>
-      <c r="F18" t="s">
-        <v>820</v>
-      </c>
-      <c r="G18" t="s">
-        <v>836</v>
-      </c>
-      <c r="H18" t="s">
-        <v>853</v>
-      </c>
-      <c r="I18" t="s">
-        <v>870</v>
-      </c>
-      <c r="J18" t="s">
-        <v>885</v>
-      </c>
-      <c r="K18" t="s">
-        <v>902</v>
-      </c>
-      <c r="L18" t="s">
-        <v>798</v>
-      </c>
-      <c r="M18" t="s">
-        <v>927</v>
-      </c>
-      <c r="N18" t="s">
-        <v>845</v>
-      </c>
-      <c r="O18" t="s">
-        <v>948</v>
-      </c>
-      <c r="P18" t="s">
-        <v>957</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>966</v>
-      </c>
-      <c r="R18" t="s">
-        <v>976</v>
-      </c>
-      <c r="S18" t="s">
-        <v>13</v>
-      </c>
-      <c r="T18" t="s">
-        <v>13</v>
-      </c>
-      <c r="U18" t="s">
-        <v>13</v>
-      </c>
-      <c r="V18" t="s">
-        <v>13</v>
-      </c>
-      <c r="W18" t="s">
-        <v>13</v>
-      </c>
-      <c r="X18" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>779</v>
-      </c>
-      <c r="D19" t="s">
-        <v>793</v>
-      </c>
-      <c r="E19" t="s">
-        <v>809</v>
-      </c>
-      <c r="F19" t="s">
-        <v>821</v>
-      </c>
-      <c r="G19" t="s">
-        <v>837</v>
-      </c>
-      <c r="H19" t="s">
-        <v>854</v>
-      </c>
-      <c r="I19" t="s">
-        <v>871</v>
-      </c>
-      <c r="J19" t="s">
-        <v>886</v>
-      </c>
-      <c r="K19" t="s">
-        <v>903</v>
-      </c>
-      <c r="L19" t="s">
-        <v>914</v>
-      </c>
-      <c r="M19" t="s">
-        <v>928</v>
-      </c>
-      <c r="N19" t="s">
-        <v>939</v>
-      </c>
-      <c r="O19" t="s">
-        <v>770</v>
-      </c>
-      <c r="P19" t="s">
-        <v>837</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>967</v>
-      </c>
-      <c r="R19" t="s">
-        <v>977</v>
-      </c>
-      <c r="S19" t="s">
-        <v>983</v>
-      </c>
-      <c r="T19" t="s">
-        <v>13</v>
-      </c>
-      <c r="U19" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" t="s">
-        <v>13</v>
-      </c>
-      <c r="W19" t="s">
-        <v>13</v>
-      </c>
-      <c r="X19" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>773</v>
-      </c>
-      <c r="D20" t="s">
-        <v>786</v>
-      </c>
-      <c r="E20" t="s">
-        <v>800</v>
-      </c>
-      <c r="F20" t="s">
-        <v>815</v>
-      </c>
-      <c r="G20" t="s">
-        <v>827</v>
-      </c>
-      <c r="H20" t="s">
-        <v>855</v>
-      </c>
-      <c r="I20" t="s">
-        <v>406</v>
-      </c>
-      <c r="J20" t="s">
-        <v>877</v>
-      </c>
-      <c r="K20" t="s">
-        <v>899</v>
-      </c>
-      <c r="L20" t="s">
-        <v>915</v>
-      </c>
-      <c r="M20" t="s">
-        <v>848</v>
-      </c>
-      <c r="N20" t="s">
-        <v>940</v>
-      </c>
-      <c r="O20" t="s">
-        <v>865</v>
-      </c>
-      <c r="P20" t="s">
-        <v>958</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>968</v>
-      </c>
-      <c r="R20" t="s">
-        <v>978</v>
-      </c>
-      <c r="S20" t="s">
-        <v>984</v>
-      </c>
-      <c r="T20" t="s">
-        <v>903</v>
-      </c>
-      <c r="U20" t="s">
-        <v>13</v>
-      </c>
-      <c r="V20" t="s">
-        <v>13</v>
-      </c>
-      <c r="W20" t="s">
-        <v>13</v>
-      </c>
-      <c r="X20" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>771</v>
-      </c>
-      <c r="D21" t="s">
-        <v>784</v>
-      </c>
-      <c r="E21" t="s">
-        <v>798</v>
-      </c>
-      <c r="F21" t="s">
-        <v>778</v>
-      </c>
-      <c r="G21" t="s">
-        <v>838</v>
-      </c>
-      <c r="H21" t="s">
-        <v>856</v>
-      </c>
-      <c r="I21" t="s">
-        <v>872</v>
-      </c>
-      <c r="J21" t="s">
-        <v>887</v>
-      </c>
-      <c r="K21" t="s">
-        <v>904</v>
-      </c>
-      <c r="L21" t="s">
-        <v>916</v>
-      </c>
-      <c r="M21" t="s">
-        <v>929</v>
-      </c>
-      <c r="N21" t="s">
-        <v>815</v>
-      </c>
-      <c r="O21" t="s">
-        <v>949</v>
-      </c>
-      <c r="P21" t="s">
-        <v>959</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>969</v>
-      </c>
-      <c r="R21" t="s">
-        <v>814</v>
-      </c>
-      <c r="S21" t="s">
-        <v>861</v>
-      </c>
-      <c r="T21" t="s">
-        <v>854</v>
-      </c>
-      <c r="U21" t="s">
-        <v>785</v>
-      </c>
-      <c r="V21" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" t="s">
-        <v>13</v>
-      </c>
-      <c r="X21" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>772</v>
-      </c>
-      <c r="D22" t="s">
-        <v>785</v>
-      </c>
-      <c r="E22" t="s">
-        <v>799</v>
-      </c>
-      <c r="F22" t="s">
-        <v>814</v>
-      </c>
-      <c r="G22" t="s">
-        <v>839</v>
-      </c>
-      <c r="H22" t="s">
-        <v>857</v>
-      </c>
-      <c r="I22" t="s">
-        <v>873</v>
-      </c>
-      <c r="J22" t="s">
-        <v>888</v>
-      </c>
-      <c r="K22" t="s">
-        <v>888</v>
-      </c>
-      <c r="L22" t="s">
-        <v>917</v>
-      </c>
-      <c r="M22" t="s">
-        <v>930</v>
-      </c>
-      <c r="N22" t="s">
-        <v>803</v>
-      </c>
-      <c r="O22" t="s">
-        <v>950</v>
-      </c>
-      <c r="P22" t="s">
-        <v>960</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>970</v>
-      </c>
-      <c r="R22" t="s">
-        <v>807</v>
-      </c>
-      <c r="S22" t="s">
-        <v>803</v>
-      </c>
-      <c r="T22" t="s">
-        <v>989</v>
-      </c>
-      <c r="U22" t="s">
-        <v>888</v>
-      </c>
-      <c r="V22" t="s">
-        <v>857</v>
-      </c>
-      <c r="W22" t="s">
-        <v>13</v>
-      </c>
-      <c r="X22" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>771</v>
-      </c>
-      <c r="D23" t="s">
-        <v>784</v>
-      </c>
-      <c r="E23" t="s">
-        <v>798</v>
-      </c>
-      <c r="F23" t="s">
-        <v>778</v>
-      </c>
-      <c r="G23" t="s">
-        <v>840</v>
-      </c>
-      <c r="H23" t="s">
-        <v>858</v>
-      </c>
-      <c r="I23" t="s">
-        <v>136</v>
-      </c>
-      <c r="J23" t="s">
-        <v>889</v>
-      </c>
-      <c r="K23" t="s">
-        <v>136</v>
-      </c>
-      <c r="L23" t="s">
-        <v>918</v>
-      </c>
-      <c r="M23" t="s">
-        <v>931</v>
-      </c>
-      <c r="N23" t="s">
-        <v>941</v>
-      </c>
-      <c r="O23" t="s">
-        <v>951</v>
-      </c>
-      <c r="P23" t="s">
-        <v>843</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>971</v>
-      </c>
-      <c r="R23" t="s">
-        <v>863</v>
-      </c>
-      <c r="S23" t="s">
-        <v>845</v>
-      </c>
-      <c r="T23" t="s">
-        <v>990</v>
-      </c>
-      <c r="U23" t="s">
-        <v>996</v>
-      </c>
-      <c r="V23" t="s">
-        <v>999</v>
-      </c>
-      <c r="W23" t="s">
-        <v>887</v>
-      </c>
-      <c r="X23" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s">
-        <v>780</v>
-      </c>
-      <c r="D24" t="s">
-        <v>794</v>
-      </c>
-      <c r="E24" t="s">
-        <v>810</v>
-      </c>
-      <c r="F24" t="s">
-        <v>822</v>
-      </c>
-      <c r="G24" t="s">
-        <v>773</v>
-      </c>
-      <c r="H24" t="s">
-        <v>859</v>
-      </c>
-      <c r="I24" t="s">
-        <v>874</v>
-      </c>
-      <c r="J24" t="s">
-        <v>890</v>
-      </c>
-      <c r="K24" t="s">
-        <v>905</v>
-      </c>
-      <c r="L24" t="s">
-        <v>919</v>
-      </c>
-      <c r="M24" t="s">
-        <v>932</v>
-      </c>
-      <c r="N24" t="s">
-        <v>942</v>
-      </c>
-      <c r="O24" t="s">
-        <v>952</v>
-      </c>
-      <c r="P24" t="s">
-        <v>961</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>972</v>
-      </c>
-      <c r="R24" t="s">
-        <v>979</v>
-      </c>
-      <c r="S24" t="s">
-        <v>985</v>
-      </c>
-      <c r="T24" t="s">
-        <v>991</v>
-      </c>
-      <c r="U24" t="s">
-        <v>997</v>
-      </c>
-      <c r="V24" t="s">
-        <v>1000</v>
-      </c>
-      <c r="W24" t="s">
-        <v>952</v>
-      </c>
-      <c r="X24" t="s">
-        <v>1005</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>781</v>
-      </c>
-      <c r="D25" t="s">
-        <v>795</v>
-      </c>
-      <c r="E25" t="s">
-        <v>811</v>
-      </c>
-      <c r="F25" t="s">
-        <v>823</v>
-      </c>
-      <c r="G25" t="s">
-        <v>841</v>
-      </c>
-      <c r="H25" t="s">
-        <v>854</v>
-      </c>
-      <c r="I25" t="s">
-        <v>825</v>
-      </c>
-      <c r="J25" t="s">
-        <v>891</v>
-      </c>
-      <c r="K25" t="s">
-        <v>886</v>
-      </c>
-      <c r="L25" t="s">
-        <v>920</v>
-      </c>
-      <c r="M25" t="s">
-        <v>836</v>
-      </c>
-      <c r="N25" t="s">
-        <v>820</v>
-      </c>
-      <c r="O25" t="s">
-        <v>770</v>
-      </c>
-      <c r="P25" t="s">
-        <v>854</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>973</v>
-      </c>
-      <c r="R25" t="s">
-        <v>980</v>
-      </c>
-      <c r="S25" t="s">
-        <v>986</v>
-      </c>
-      <c r="T25" t="s">
-        <v>992</v>
-      </c>
-      <c r="U25" t="s">
-        <v>886</v>
-      </c>
-      <c r="V25" t="s">
-        <v>779</v>
-      </c>
-      <c r="W25" t="s">
-        <v>1002</v>
-      </c>
-      <c r="X25" t="s">
-        <v>1006</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>894</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>772</v>
-      </c>
-      <c r="D26" t="s">
-        <v>785</v>
-      </c>
-      <c r="E26" t="s">
-        <v>799</v>
-      </c>
-      <c r="F26" t="s">
-        <v>814</v>
-      </c>
-      <c r="G26" t="s">
-        <v>812</v>
-      </c>
-      <c r="H26" t="s">
-        <v>860</v>
-      </c>
-      <c r="I26" t="s">
-        <v>875</v>
-      </c>
-      <c r="J26" t="s">
-        <v>892</v>
-      </c>
-      <c r="K26" t="s">
-        <v>906</v>
-      </c>
-      <c r="L26" t="s">
-        <v>921</v>
-      </c>
-      <c r="M26" t="s">
-        <v>933</v>
-      </c>
-      <c r="N26" t="s">
-        <v>943</v>
-      </c>
-      <c r="O26" t="s">
-        <v>953</v>
-      </c>
-      <c r="P26" t="s">
-        <v>962</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>974</v>
-      </c>
-      <c r="R26" t="s">
-        <v>981</v>
-      </c>
-      <c r="S26" t="s">
-        <v>893</v>
-      </c>
-      <c r="T26" t="s">
-        <v>993</v>
-      </c>
-      <c r="U26" t="s">
-        <v>801</v>
-      </c>
-      <c r="V26" t="s">
-        <v>1001</v>
-      </c>
-      <c r="W26" t="s">
-        <v>1003</v>
-      </c>
-      <c r="X26" t="s">
-        <v>1007</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>1009</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>1012</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>778</v>
-      </c>
-      <c r="D27" t="s">
-        <v>792</v>
-      </c>
-      <c r="E27" t="s">
-        <v>808</v>
-      </c>
-      <c r="F27" t="s">
-        <v>820</v>
-      </c>
-      <c r="G27" t="s">
-        <v>836</v>
-      </c>
-      <c r="H27" t="s">
-        <v>861</v>
-      </c>
-      <c r="I27" t="s">
-        <v>876</v>
-      </c>
-      <c r="J27" t="s">
-        <v>893</v>
-      </c>
-      <c r="K27" t="s">
-        <v>907</v>
-      </c>
-      <c r="L27" t="s">
-        <v>922</v>
-      </c>
-      <c r="M27" t="s">
-        <v>934</v>
-      </c>
-      <c r="N27" t="s">
-        <v>944</v>
-      </c>
-      <c r="O27" t="s">
-        <v>954</v>
-      </c>
-      <c r="P27" t="s">
-        <v>963</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>967</v>
-      </c>
-      <c r="R27" t="s">
-        <v>982</v>
-      </c>
-      <c r="S27" t="s">
-        <v>987</v>
-      </c>
-      <c r="T27" t="s">
-        <v>994</v>
-      </c>
-      <c r="U27" t="s">
-        <v>907</v>
-      </c>
-      <c r="V27" t="s">
-        <v>861</v>
-      </c>
-      <c r="W27" t="s">
-        <v>858</v>
-      </c>
-      <c r="X27" t="s">
-        <v>876</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>1010</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>1013</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>803</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" t="s">
-        <v>782</v>
-      </c>
-      <c r="D28" t="s">
-        <v>796</v>
-      </c>
-      <c r="E28" t="s">
-        <v>812</v>
-      </c>
-      <c r="F28" t="s">
-        <v>824</v>
-      </c>
-      <c r="G28" t="s">
-        <v>842</v>
-      </c>
-      <c r="H28" t="s">
-        <v>862</v>
-      </c>
-      <c r="I28" t="s">
-        <v>783</v>
-      </c>
-      <c r="J28" t="s">
-        <v>894</v>
-      </c>
-      <c r="K28" t="s">
-        <v>908</v>
-      </c>
-      <c r="L28" t="s">
-        <v>923</v>
-      </c>
-      <c r="M28" t="s">
-        <v>834</v>
-      </c>
-      <c r="N28" t="s">
-        <v>781</v>
-      </c>
-      <c r="O28" t="s">
-        <v>955</v>
-      </c>
-      <c r="P28" t="s">
-        <v>964</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>975</v>
-      </c>
-      <c r="R28" t="s">
-        <v>837</v>
-      </c>
-      <c r="S28" t="s">
-        <v>988</v>
-      </c>
-      <c r="T28" t="s">
-        <v>995</v>
-      </c>
-      <c r="U28" t="s">
-        <v>998</v>
-      </c>
-      <c r="V28" t="s">
-        <v>770</v>
-      </c>
-      <c r="W28" t="s">
-        <v>1004</v>
-      </c>
-      <c r="X28" t="s">
-        <v>1008</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>1011</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>1014</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>1015</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>